<commit_message>
Content published for CMS applications
</commit_message>
<xml_diff>
--- a/documents/common-component-matrix.xlsx
+++ b/documents/common-component-matrix.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\DFE\Top15\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\github\architecture\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AA99E81D-BD3E-4D7C-9BEE-B53C5EF7943F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{468E4FD6-4EF3-4E1B-9738-18386FA8E02D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9060" yWindow="1740" windowWidth="25170" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25320" yWindow="-120" windowWidth="25440" windowHeight="15390" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping Applications" sheetId="1" r:id="rId1"/>
     <sheet name="Mapping Services" sheetId="4" r:id="rId2"/>
     <sheet name="Postcode Applications" sheetId="5" r:id="rId3"/>
     <sheet name="Postcode Services" sheetId="6" r:id="rId4"/>
-    <sheet name="Notification Application" sheetId="7" r:id="rId5"/>
+    <sheet name="Notification Applications" sheetId="7" r:id="rId5"/>
     <sheet name="Notification Services" sheetId="8" r:id="rId6"/>
+    <sheet name="CMS Applications" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -1263,7 +1264,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="991" uniqueCount="431">
   <si>
     <t>Azure Maps</t>
   </si>
@@ -2051,12 +2052,742 @@
   <si>
     <t>https://dfedigital.atlassian.net/wiki/spaces/TSTL/pages/1223458929/What+we+use+and+defaults</t>
   </si>
+  <si>
+    <t>Feature</t>
+  </si>
+  <si>
+    <t>Contentful</t>
+  </si>
+  <si>
+    <t>Contentstack</t>
+  </si>
+  <si>
+    <t>Kontent</t>
+  </si>
+  <si>
+    <t>Prismic</t>
+  </si>
+  <si>
+    <t>Cosmic JS</t>
+  </si>
+  <si>
+    <t>Sitefinity</t>
+  </si>
+  <si>
+    <t>OrchardCore</t>
+  </si>
+  <si>
+    <t>Weblink</t>
+  </si>
+  <si>
+    <t>https://www.contentful.com/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.contentstack.com/ </t>
+  </si>
+  <si>
+    <t>https://kontent.ai/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://prismic.io/ </t>
+  </si>
+  <si>
+    <t>https://www.cosmicjs.com/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.progress.com/sitefinity-cms </t>
+  </si>
+  <si>
+    <t>http://www.orchardcore.net/</t>
+  </si>
+  <si>
+    <t>Licence Type/Pricing Structure</t>
+  </si>
+  <si>
+    <t>Dependent on usecases, specific requirements (inc. specialist language content) and size of service</t>
+  </si>
+  <si>
+    <t>•	On-demand = Pay for the space only
+•	Micro = €420/year (1 master and 1 sandbox environment, 1 role, 2 locales, 24 content types, 5,000 records)
+•	Small = €2,028/year (1 master and 2 sandbox environment, 2 role, 4 locales, 24 content types, 10,000 records)
+•	Medium = €5,268/year (1 master and 3 sandbox environment, 2 role, 7 locales, 48 content types, 25,000 records)
+•	Large = €9,468/year (1 master and 5 sandbox environment, 4 role, 10 locales, 48 content types, 50,000 records, plus GraphQL API)
+•	Enterprise = Pay for the platform + SLA + space
+•	Professional = €24,000+/year (+ space and SLA costs) - custom roles, SSO, full webhook functionality, scheduled publishing
+•	Scale = €90,000+/year (+ space and SLA costs)
+•	High availability = €225,000+/year (+ space and SLA costs)</t>
+  </si>
+  <si>
+    <t>•Business = $3,500/month
+-10 Users
+- 1 Property
+- Content Types
+- Digital Assets Management
+- Rich Text Editor
+- Multiple Environments
+- Modular Blocks (Page Builder)
+- Custom Fields
+•Enterprise = Starts at $10,000/month (requires quotation) and onboarding fee required for first year
+- 10+ Users
+- 3+ Properties
+- Workflows
+- Grouped Releases
+- Bulk Operations
+- Experience Extensions (Integrations)
+- Dashboard
+- Analytics</t>
+  </si>
+  <si>
+    <t>•Starter = Free
+- 3 Users ($10/month per extra user. Max 20 users)
+- Unlimited projects (but without ability to clone)
+- 5,000 Content items
+- 2 Languages
+•Business = $999/month
+- 15 Users ($10/month per extra user. Max 30 users)
+- Unlimited projects
+- 25,000 Content items
+- 10 Languages
+- 1 predefined role + 2 Custom roles
+•Enterprise = Starts at $1,499/month (requires quotation)
+- Custom number of Users
+- Unlimited projects
+- More Content items
+- More Languages
+- More Custom roles</t>
+  </si>
+  <si>
+    <t>•Free and Starter are the cheapest tiers
+•Small = $20/month OR $15/month for annual contract
+- 7 Users
+- Basic Support
+- Core features
+•Professional - Medium = $125/month OR $100/month for annual contract
+- 25 Users
+- SLA (99,5% API Uptime), Basic Support
+- User roles, publication workflow &amp; collaboration features
+•Professional - Platinum = $575/month OR $500/month for annual contract
+- Unlimited users
+- SLA (99,5% API Uptime), Priority Support
+- User roles, publication workflow &amp; collaboration features
+•Enterprise = Starts at $24,000/year (requires quotation)
+- Includes three environments (development, staging, production)
+- SLA (99.95% API Uptime)
+- Daily backups &amp; snapshots
+- SSO and MFA</t>
+  </si>
+  <si>
+    <t>•	Personal Plan provides a free option
+•	Starter = $99/month (10% off for annual)
+- Single Bucket
+- 5 team members
+- 25,000 API requests
+- 10,000 files / 3GB media storage
+•	Pro = $299/month (10% off for annual)
+- Single Bucket
+- 10 team members
+- 150,000 API requests
+- 50,000 files / 15GB media storage
+•	Business = $799/month (10% off for annual)
+- Single Bucket
+- 30 team members
+- 500,000 API requests
+- 100,000 files / 50GB media storage
+•	Enterprise = requires quotation
+- Dedicated Infrastructure
+- Single Sign-on
+- 24/7 Support
+- SLA
+- Migration Support
+- All add-ons included
+- Company workspace</t>
+  </si>
+  <si>
+    <t>•	Professional Edition = Starts at $15,000/year (requires quotation)
+- 1 production domain or server
+- 10 concurrent users
+- Web Content Management
+- Developer Productivity Tools
+•	Online Marketing Edition = Starts at $30,000+/year (requires quotation)
+- 1 production domain
+- 15 concurrent users
+- Web Content Management
+- Developer Productivity Tools
+- Marketing and CRM connectors
+- Content personalisation
+•	Enterprise Edition = Starts at $50,000/year (requires quotation)
+- Unlimited concurrent users
+- Web Content Management
+- Developer Productivity Tools
+- All connectors
+- Content personalisation
+- Site sync between environments
+- Translations management
+- System audit trail</t>
+  </si>
+  <si>
+    <t>Opensource</t>
+  </si>
+  <si>
+    <t>Service Type</t>
+  </si>
+  <si>
+    <t>Cloud based or on Prem</t>
+  </si>
+  <si>
+    <t>As a product owner I want a CMS service to develop content so that I can publish digital content online.</t>
+  </si>
+  <si>
+    <t>SaaS</t>
+  </si>
+  <si>
+    <t>PaaS</t>
+  </si>
+  <si>
+    <t>Compatible with Ruby on Rails</t>
+  </si>
+  <si>
+    <t>As a product owner I want….</t>
+  </si>
+  <si>
+    <t>N 
+(.Net platform)</t>
+  </si>
+  <si>
+    <t>Restful API</t>
+  </si>
+  <si>
+    <t>Allows it to communicate with other services and components, using best practice protocols</t>
+  </si>
+  <si>
+    <t>As a product owner I want the CMS to be interoperable with other component and services so that the platform is extensible.</t>
+  </si>
+  <si>
+    <t>Graph QL</t>
+  </si>
+  <si>
+    <t>Query language for APIs</t>
+  </si>
+  <si>
+    <t>As a product owner I want be able to query the data held within the CMS so that I can search for specific information.</t>
+  </si>
+  <si>
+    <t>Supports webhooks</t>
+  </si>
+  <si>
+    <t>Provide real-time event driven information</t>
+  </si>
+  <si>
+    <t>As a product owner I want to use webhooks for my app or platform so that I can provide a real-time without developing an AP.</t>
+  </si>
+  <si>
+    <t>Y
+- Webhooks supported but functionality is limited below Enterprise level (e.g. not possible to trigger a webhook off certain "event" types). Templates and static webhook IPs provided in Enterprise version.</t>
+  </si>
+  <si>
+    <t>Integrations</t>
+  </si>
+  <si>
+    <t>Ability to interface and connect with other platforms and services</t>
+  </si>
+  <si>
+    <t>API</t>
+  </si>
+  <si>
+    <t>API
+- Integrates with martech technologies such as Marketo, Salesforce, Google Analytics, SEMrush, Brightcove, Watson, etc.
+- Integrations with Google Docs and Slack are being developed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+- Integration with task management tools such as Trello, Jira and Asana in the roadmap
+- Delivery API not exposed in free Starter version.</t>
+  </si>
+  <si>
+    <t>API
+- Integrations with Slack being discussed but still in the roadmap</t>
+  </si>
+  <si>
+    <t>API
+-Integration with a number of web services including Slack, GitHub, Google Analytics</t>
+  </si>
+  <si>
+    <t>Integrated with NEO for GraghQL interface/ Sparql (WC3 standard)</t>
+  </si>
+  <si>
+    <t>Notifications</t>
+  </si>
+  <si>
+    <t>Ability to send and receive messages in different applications</t>
+  </si>
+  <si>
+    <t>As a product owner I want to be able to send messages from the CMS so other platforms or service so that I can communicate with users.</t>
+  </si>
+  <si>
+    <t>Y
+- Notifications work in Slack as well as email</t>
+  </si>
+  <si>
+    <t>Content Previewing</t>
+  </si>
+  <si>
+    <t>To be able to preview content before it is published online</t>
+  </si>
+  <si>
+    <t>As a product owner I want I want to view my content before it is published online so that I can validate it is correct.</t>
+  </si>
+  <si>
+    <t>Rich Text Format Editor</t>
+  </si>
+  <si>
+    <t>Text formatting options</t>
+  </si>
+  <si>
+    <t>As a product owner I want to be able to format the text so that it is accessible for the audience.</t>
+  </si>
+  <si>
+    <t>Version History</t>
+  </si>
+  <si>
+    <t>To be able number and keep a log of historic releases</t>
+  </si>
+  <si>
+    <t>As a product owner I want to be able to view the history of published changes so that I have a record of past versions.</t>
+  </si>
+  <si>
+    <t>Scheduled Publishing</t>
+  </si>
+  <si>
+    <t>Ability to set the time content is to be published</t>
+  </si>
+  <si>
+    <t>As a product owner I want develop and release content at a plannned time so that content is published at the scheduled time.</t>
+  </si>
+  <si>
+    <t>Publishing Approval Workflow</t>
+  </si>
+  <si>
+    <t>Automated approval sign off for content before it is published</t>
+  </si>
+  <si>
+    <t>As a product owner I want changes to content to go through a business approval process so that the necessary checks are in place before publishing.</t>
+  </si>
+  <si>
+    <t>Workflow Tools</t>
+  </si>
+  <si>
+    <t>Ability to define processes and workflows to create, approve and publish content</t>
+  </si>
+  <si>
+    <t>- Content approval Workflows
+- Notifications only available in Enterprise plans
+- Custom roles only available in Enterprise plans
+- Content publishing and expiry scheduling only available in Enterprise plans
+- Content versioning and revision history for all plans</t>
+  </si>
+  <si>
+    <t>- Content publishing and expiry scheduling for all plans
+- Versioning and rollback
+- Built in approval workflows only available in Enterprise version
+- Ability to use webhooks for notifications limited below Enterprise
+- Grouped releases only available in Enterprise version</t>
+  </si>
+  <si>
+    <t>- Request review and approve content workflow (excluding free version)
+- Ability to leave comments and suggest changes for approval (excluding free version)
+- Built in notifications tool (email and Slack)
+- No limit on how webhooks are used for notifications
+- Revision history
+- Content publishing and expiry scheduling (excluding free version)
+- Dashboard view of assignments
+- Calendar view to see upcoming publishing or content expiry dates</t>
+  </si>
+  <si>
+    <t>- User roles limited to three (admin, publisher, writer) with no custom roles
+- Publishing workflow tool available in all plans
+- No limits on how webhooks are used for notifications
+- Release scheduling and bulk publishing for all plans
+- Full revision history</t>
+  </si>
+  <si>
+    <t>- Ability to build content publishing workflow for all plans
+- Zapier used for notifications
+- Scheduled publishing and expiry for all plans
+- Revision history for all plans</t>
+  </si>
+  <si>
+    <t>- Approval workflow tools and user permissions
+- Built in email notification tool
+- No limits on how webhooks are used for notifications
+- Content Publication &amp; Expiration Scheduling for all plans</t>
+  </si>
+  <si>
+    <t>Can develop and edit workflows</t>
+  </si>
+  <si>
+    <t>Multimedia Capability</t>
+  </si>
+  <si>
+    <t>Ability to Support media files such as images, videos, sound files etc</t>
+  </si>
+  <si>
+    <t>As a product owner I want to publish multimedia content so that I can give a rich user experience to the user.</t>
+  </si>
+  <si>
+    <t>- Wide variety of content modelling options- content types include text, dates, rich text, media (images, docs etc.), location, references to other content, arrays and even JSON for data.</t>
+  </si>
+  <si>
+    <t>- Supports all media files such as image link, video link, GIFs etc.
+- Maximum size of a single asset file is 700 MB (this can be restricted further using validation rules).</t>
+  </si>
+  <si>
+    <t>- Asset library supports a range of media types</t>
+  </si>
+  <si>
+    <t>- Every repository on Prismic has its own media library, which supports a range of file types including images, sounds files, videos, pdfs and more.
+- Max image size is 10Mb and max for any other file type is 100Mb
+- Imgix API used to make builds with images easier</t>
+  </si>
+  <si>
+    <t>- Supports a wide variety of media types including video.</t>
+  </si>
+  <si>
+    <t>No image manipulaton/ can use CDL</t>
+  </si>
+  <si>
+    <t>Secure Hosting</t>
+  </si>
+  <si>
+    <t>Hosting that is encrypted at rest and intransit and accessed securley (physical and digital). And hosted in a secure location.</t>
+  </si>
+  <si>
+    <t>As a product owner I want a secure service so that I can deliver content that is security compliant.</t>
+  </si>
+  <si>
+    <t>- Use AWS hosting</t>
+  </si>
+  <si>
+    <t>Multifactor Authentication</t>
+  </si>
+  <si>
+    <t>Enhanced authentication capability</t>
+  </si>
+  <si>
+    <t>As a product owner I want to keep access to the CMS platform secure so that only authorised user can access the platform.</t>
+  </si>
+  <si>
+    <t>Y
+- 2FA is an option even for the free tier but it is not enforced</t>
+  </si>
+  <si>
+    <t>Y
+For Enterprise Plans</t>
+  </si>
+  <si>
+    <t>Y
+Two factor authentication for Enterprise plans</t>
+  </si>
+  <si>
+    <t>- Two-factor authentication included for all plans.</t>
+  </si>
+  <si>
+    <t>- Windows and other authenticator options</t>
+  </si>
+  <si>
+    <t>Requires development and integration into identity provider</t>
+  </si>
+  <si>
+    <t>Security Certification</t>
+  </si>
+  <si>
+    <t>Provider is compliant with required standards</t>
+  </si>
+  <si>
+    <t>As a product owner I want the assurance that the CMS platform provider can demonstrate security compliance so that I know the platform will be secure to deliver my service.</t>
+  </si>
+  <si>
+    <t>Y 
+(ISO 27001:2013 compliant and ISO 27001 compliant data centres)</t>
+  </si>
+  <si>
+    <t>Y
+- SOC 2 Type II certification
+- ISO 27001 Compliant Data Centres - North American &amp; European Datacentres</t>
+  </si>
+  <si>
+    <t>- ISO 9001:2015, ISO 27001:2013 and ISO 20000-1:2011 certifications</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ISO/IEC 27001:2013, ISO/IEC 27017</t>
+  </si>
+  <si>
+    <t>- No ISO certifications</t>
+  </si>
+  <si>
+    <t>- Microsoft Azure infrastructure with ISO/IEC 27018, SOC 2 and more certifications</t>
+  </si>
+  <si>
+    <t>Pen tested by Fidus</t>
+  </si>
+  <si>
+    <t>Custom Roles</t>
+  </si>
+  <si>
+    <t>Ability to granularly control user access</t>
+  </si>
+  <si>
+    <t>As a product owner I want to be able to define user roles and permissions so that I can control levels of access to the CMS platform.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Custom roles only available in Enterprise plans</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Y
+In all plans
+</t>
+  </si>
+  <si>
+    <t>Custom roles for all plans</t>
+  </si>
+  <si>
+    <t>Pen Testing</t>
+  </si>
+  <si>
+    <t>Validate that that service has undertaken security assurances</t>
+  </si>
+  <si>
+    <t>As a product owner I want to know that the platform is regularly assessed for risks and vulnerabilities so that I know it is secure to deliver my service.</t>
+  </si>
+  <si>
+    <t>Y 
+(annual)</t>
+  </si>
+  <si>
+    <t>Y
+- Biannual Vulnerability Assessment and Penetration Testing (VAPT)</t>
+  </si>
+  <si>
+    <t>Annually</t>
+  </si>
+  <si>
+    <t>SSO</t>
+  </si>
+  <si>
+    <t>Ability to integrate with other identity services (e.g SAML 2.0 or Oauth)</t>
+  </si>
+  <si>
+    <t>As a product owner I want to be able to integrate my organisational SSO with the CMS platform so that users can use their corporate identity to access the platorm.</t>
+  </si>
+  <si>
+    <t>Only for enterprise plan</t>
+  </si>
+  <si>
+    <t>SSO with SAML 2.0</t>
+  </si>
+  <si>
+    <t>Single Sign-On for Enterprise plans</t>
+  </si>
+  <si>
+    <t>- Single-Sign-On for all plans</t>
+  </si>
+  <si>
+    <t>Third party sign on</t>
+  </si>
+  <si>
+    <t>Encryption (transit and rest)</t>
+  </si>
+  <si>
+    <t>Ensure all data is securley encrypted in transit and at rest (e.g TLS 1.2)</t>
+  </si>
+  <si>
+    <t>As a product owner I want to keep data secure when being transferred over a network so that we minimise data breaches and risk.</t>
+  </si>
+  <si>
+    <t>Y
+- 256-bit encryption of data in transit and at rest</t>
+  </si>
+  <si>
+    <t>- Data transferred between Prismic AWS EC2 instances and S3 storage facilities is secured via SSL endpoints using the HTTPS protocol. all Content Data is stored On disks in an encrypted manner (encrypted at rest)</t>
+  </si>
+  <si>
+    <t>- Data encryption at rest with 256-bit SSL encryption in transit</t>
+  </si>
+  <si>
+    <t>- Data transfer encryption (TLS 1.2)</t>
+  </si>
+  <si>
+    <t>Security Reporting</t>
+  </si>
+  <si>
+    <t>Insight report into security status and vulnerabilities of the service</t>
+  </si>
+  <si>
+    <t>As a product owner I want regular reports about the security health of the CMS platform so that I know it is secure and that vulnerabilities can be addressed.</t>
+  </si>
+  <si>
+    <t>Usage and activity reports</t>
+  </si>
+  <si>
+    <t>Uses Azure Monitoring</t>
+  </si>
+  <si>
+    <t>Data Soverignty</t>
+  </si>
+  <si>
+    <t>Location where the data is hosted and is subject to location data processsing policy and laws (e.g. GDPR)</t>
+  </si>
+  <si>
+    <t>As a product owner I want my service to be hosted in a secure compliant regional location so that I know my data and service will be secure by laws.</t>
+  </si>
+  <si>
+    <t>USA (Primary) &amp; EU (Backup)
+- Data is all hosted in North America, which could be an issue for any sensitive content</t>
+  </si>
+  <si>
+    <t>EU &amp; USA</t>
+  </si>
+  <si>
+    <t>Can choose - EU/USA/AUS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Data hosted in AWS facilities in Virginia, USA </t>
+  </si>
+  <si>
+    <t>Multi Region</t>
+  </si>
+  <si>
+    <t>On own infrastructure</t>
+  </si>
+  <si>
+    <t>Customer Support</t>
+  </si>
+  <si>
+    <t>First-line and technical support offered to the  organisation</t>
+  </si>
+  <si>
+    <t>As a product owner I want helpdesk support for the CMS platform so that if there any technical issues I can access support.</t>
+  </si>
+  <si>
+    <t>- Direct support only available for Enterprise plans.</t>
+  </si>
+  <si>
+    <t>Y
+- All Contentstack customers receive 24hr (Mon-Fri) support with average response times under 5 minutes. Enterprise plan includes 24/7 support.</t>
+  </si>
+  <si>
+    <t>Y
+- Priority chat and email for Business plan and 24/7x365 chat, email and phone for Enterprise
+- Service availability starts at 99.5% for Enterprise plans</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Y
+Priority Support in Platinum plan
+</t>
+  </si>
+  <si>
+    <t>-16h/day (Mon-Fri) in Professional plan</t>
+  </si>
+  <si>
+    <t>Y 
+(Community support)</t>
+  </si>
+  <si>
+    <t>Usability</t>
+  </si>
+  <si>
+    <t>Intuitive and easy to use with mininal training, configurable and accessible for users.</t>
+  </si>
+  <si>
+    <t>As a product owner I want the CMS platform to be easy to use so that I don't need specialist support.</t>
+  </si>
+  <si>
+    <t>- Simple to use WYSIWYG rich text editor
+- Simple content previewing</t>
+  </si>
+  <si>
+    <t>- WYSIWYG rich text editor
+- Content previewing requires publishing to a  "Preview" environment rather than there being a one click preview option (reducing the ease slightly)</t>
+  </si>
+  <si>
+    <t>- WYSIWYG rich text editor
+- Content previewing with in-browser editing</t>
+  </si>
+  <si>
+    <t>- WYSIWYG rich text editor
+- Drag and drop visual editing
+- Content previewing with in-browser editing feature
+- Page tagging and filtering</t>
+  </si>
+  <si>
+    <t>- WYSIWYG rich text editor
+- Content previewing</t>
+  </si>
+  <si>
+    <t>- WYSIWYG rich text editor
+- Content previewing including mobile devices
+- Drag and drop visual editing
+- Clean Copy &amp; Paste from Microsoft Word</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- WYSIWYG rich text editor
+</t>
+  </si>
+  <si>
+    <t>Uptime SLA's</t>
+  </si>
+  <si>
+    <t>Availablity and reliability of the service and how quick it is to recover and restore from and outage</t>
+  </si>
+  <si>
+    <t>As a product owner I want the CMS platform to have high availablity so that I can avoid a loss of service or downtime.</t>
+  </si>
+  <si>
+    <t>Y
+- SLA (99,9% API Uptime) 
+- 99.95% of API Uptime in Enterprise version</t>
+  </si>
+  <si>
+    <t>Y (99.9%)</t>
+  </si>
+  <si>
+    <t>PaaS dependent (by design)</t>
+  </si>
+  <si>
+    <t>Other Factors</t>
+  </si>
+  <si>
+    <t>Prices competitive at the mid and enterprise levels. Kontent is an option to give further consideration if looking to invest in the additional functionality that comes with a more premium plan.</t>
+  </si>
+  <si>
+    <t>Lack of ISO certifications rule this vendor out as an option at present. But the prices and features appear very competitive at this mid-level so Cosmic JS may be an option to reconsider in the future.</t>
+  </si>
+  <si>
+    <t>Not compatible with Ruby on Rails (.NET platform).
+Seems to be a decoupled rather than "API-first" headless CMS</t>
+  </si>
+  <si>
+    <t>Existing DfE Experience</t>
+  </si>
+  <si>
+    <t>As a product owner I want to reuse existing CMS patterns, templates and workflows so that I minimise the development time for my service.</t>
+  </si>
+  <si>
+    <t>-ILR
+-Apprenticeship Fire it up
+-Service Manual team</t>
+  </si>
+  <si>
+    <t>No known experience.</t>
+  </si>
+  <si>
+    <t>Used by National Careers Service team.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2141,6 +2872,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -2195,7 +2934,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2340,6 +3079,63 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2624,23 +3420,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" customWidth="1"/>
-    <col min="2" max="2" width="29.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.28515625" style="14" customWidth="1"/>
-    <col min="4" max="4" width="68.85546875" style="14" customWidth="1"/>
+    <col min="1" max="1" width="5.44140625" customWidth="1"/>
+    <col min="2" max="2" width="29.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.33203125" style="14" customWidth="1"/>
+    <col min="4" max="4" width="68.88671875" style="14" customWidth="1"/>
     <col min="5" max="5" width="12" style="12" customWidth="1"/>
-    <col min="6" max="6" width="23.28515625" customWidth="1"/>
-    <col min="7" max="7" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.7109375" customWidth="1"/>
+    <col min="6" max="6" width="23.33203125" customWidth="1"/>
+    <col min="7" max="7" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
       <c r="F2" s="3" t="s">
         <v>0</v>
       </c>
@@ -2651,7 +3447,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B3" s="16" t="s">
         <v>3</v>
       </c>
@@ -2668,7 +3464,7 @@
       <c r="G3" s="2"/>
       <c r="H3" s="32"/>
     </row>
-    <row r="4" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B4" s="17" t="s">
         <v>7</v>
       </c>
@@ -2691,7 +3487,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B5" s="17" t="s">
         <v>12</v>
       </c>
@@ -2714,7 +3510,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B6" s="17" t="s">
         <v>16</v>
       </c>
@@ -2737,7 +3533,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B7" s="17" t="s">
         <v>21</v>
       </c>
@@ -2760,7 +3556,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B8" s="17" t="s">
         <v>24</v>
       </c>
@@ -2783,7 +3579,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B9" s="17" t="s">
         <v>27</v>
       </c>
@@ -2806,7 +3602,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B10" s="17" t="s">
         <v>30</v>
       </c>
@@ -2829,7 +3625,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B11" s="19" t="s">
         <v>33</v>
       </c>
@@ -2840,7 +3636,7 @@
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
     </row>
-    <row r="12" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B12" s="17" t="s">
         <v>34</v>
       </c>
@@ -2863,7 +3659,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B13" s="17" t="s">
         <v>38</v>
       </c>
@@ -2886,7 +3682,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B14" s="17" t="s">
         <v>41</v>
       </c>
@@ -2909,7 +3705,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B15" s="17" t="s">
         <v>44</v>
       </c>
@@ -2932,7 +3728,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B16" s="17" t="s">
         <v>48</v>
       </c>
@@ -2955,7 +3751,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="17" t="s">
         <v>51</v>
       </c>
@@ -2978,7 +3774,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B18" s="17" t="s">
         <v>53</v>
       </c>
@@ -3001,7 +3797,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B19" s="17" t="s">
         <v>55</v>
       </c>
@@ -3024,7 +3820,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B20" s="19" t="s">
         <v>58</v>
       </c>
@@ -3035,7 +3831,7 @@
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
     </row>
-    <row r="21" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B21" s="17" t="s">
         <v>59</v>
       </c>
@@ -3058,7 +3854,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B22" s="17" t="s">
         <v>62</v>
       </c>
@@ -3081,7 +3877,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B23" s="17" t="s">
         <v>65</v>
       </c>
@@ -3104,7 +3900,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B24" s="17" t="s">
         <v>68</v>
       </c>
@@ -3127,7 +3923,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B25" s="17" t="s">
         <v>71</v>
       </c>
@@ -3150,7 +3946,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="2:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B26" s="17" t="s">
         <v>74</v>
       </c>
@@ -3173,7 +3969,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B27" s="17" t="s">
         <v>77</v>
       </c>
@@ -3196,7 +3992,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B28" s="17" t="s">
         <v>80</v>
       </c>
@@ -3219,7 +4015,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>83</v>
       </c>
@@ -3230,7 +4026,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>86</v>
       </c>
@@ -3256,21 +4052,21 @@
       <selection activeCell="K43" sqref="K43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="3" width="35.85546875" customWidth="1"/>
-    <col min="4" max="5" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="35.88671875" customWidth="1"/>
+    <col min="4" max="5" width="28.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.7109375" customWidth="1"/>
+    <col min="7" max="7" width="24.6640625" customWidth="1"/>
     <col min="8" max="8" width="33" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="44.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.5703125" customWidth="1"/>
-    <col min="12" max="12" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="44.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.5546875" customWidth="1"/>
+    <col min="12" max="12" width="33.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="35.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.3">
       <c r="D2" s="5" t="s">
         <v>88</v>
       </c>
@@ -3302,7 +4098,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>97</v>
       </c>
@@ -3322,7 +4118,7 @@
       <c r="L3" s="7"/>
       <c r="M3" s="7"/>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>100</v>
       </c>
@@ -3358,7 +4154,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>102</v>
       </c>
@@ -3394,7 +4190,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
@@ -3410,7 +4206,7 @@
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
@@ -3426,7 +4222,7 @@
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
         <v>16</v>
       </c>
@@ -3446,7 +4242,7 @@
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
         <v>21</v>
       </c>
@@ -3466,7 +4262,7 @@
       <c r="L9" s="4"/>
       <c r="M9" s="4"/>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
         <v>24</v>
       </c>
@@ -3486,7 +4282,7 @@
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
         <v>27</v>
       </c>
@@ -3506,7 +4302,7 @@
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
         <v>30</v>
       </c>
@@ -3526,7 +4322,7 @@
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
         <v>33</v>
       </c>
@@ -3542,7 +4338,7 @@
       <c r="L13" s="5"/>
       <c r="M13" s="5"/>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
         <v>34</v>
       </c>
@@ -3562,7 +4358,7 @@
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
         <v>38</v>
       </c>
@@ -3582,7 +4378,7 @@
       <c r="L15" s="4"/>
       <c r="M15" s="4"/>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
         <v>41</v>
       </c>
@@ -3598,7 +4394,7 @@
       <c r="L16" s="4"/>
       <c r="M16" s="4"/>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
         <v>44</v>
       </c>
@@ -3614,7 +4410,7 @@
       <c r="L17" s="4"/>
       <c r="M17" s="4"/>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
         <v>48</v>
       </c>
@@ -3630,7 +4426,7 @@
       <c r="L18" s="4"/>
       <c r="M18" s="4"/>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
         <v>51</v>
       </c>
@@ -3646,7 +4442,7 @@
       <c r="L19" s="4"/>
       <c r="M19" s="4"/>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
         <v>53</v>
       </c>
@@ -3662,7 +4458,7 @@
       <c r="L20" s="4"/>
       <c r="M20" s="4"/>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
         <v>55</v>
       </c>
@@ -3682,7 +4478,7 @@
       <c r="L21" s="4"/>
       <c r="M21" s="4"/>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B22" s="2" t="s">
         <v>58</v>
       </c>
@@ -3698,7 +4494,7 @@
       <c r="L22" s="5"/>
       <c r="M22" s="5"/>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B23" s="1" t="s">
         <v>59</v>
       </c>
@@ -3714,7 +4510,7 @@
       <c r="L23" s="4"/>
       <c r="M23" s="4"/>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B24" s="1" t="s">
         <v>62</v>
       </c>
@@ -3734,7 +4530,7 @@
       <c r="L24" s="4"/>
       <c r="M24" s="4"/>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B25" s="1" t="s">
         <v>65</v>
       </c>
@@ -3754,7 +4550,7 @@
       <c r="L25" s="4"/>
       <c r="M25" s="4"/>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B26" s="1" t="s">
         <v>68</v>
       </c>
@@ -3770,7 +4566,7 @@
       <c r="L26" s="4"/>
       <c r="M26" s="4"/>
     </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B27" s="1" t="s">
         <v>71</v>
       </c>
@@ -3786,7 +4582,7 @@
       <c r="L27" s="4"/>
       <c r="M27" s="4"/>
     </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B28" s="1" t="s">
         <v>74</v>
       </c>
@@ -3802,7 +4598,7 @@
       <c r="L28" s="4"/>
       <c r="M28" s="4"/>
     </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B29" s="1" t="s">
         <v>77</v>
       </c>
@@ -3818,7 +4614,7 @@
       <c r="L29" s="4"/>
       <c r="M29" s="4"/>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B30" s="1" t="s">
         <v>80</v>
       </c>
@@ -3834,7 +4630,7 @@
       <c r="L30" s="4"/>
       <c r="M30" s="4"/>
     </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B31" s="2" t="s">
         <v>106</v>
       </c>
@@ -3850,7 +4646,7 @@
       <c r="L31" s="9"/>
       <c r="M31" s="9"/>
     </row>
-    <row r="32" spans="2:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:13" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="11" t="s">
         <v>107</v>
       </c>
@@ -3891,20 +4687,20 @@
       <selection activeCell="F4" sqref="F4:F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.42578125" style="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" style="27" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.28515625" customWidth="1"/>
-    <col min="8" max="9" width="24.7109375" customWidth="1"/>
-    <col min="10" max="10" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.7109375" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.6640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.44140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" style="27" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.33203125" customWidth="1"/>
+    <col min="8" max="9" width="24.6640625" customWidth="1"/>
+    <col min="10" max="10" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
       <c r="F2" s="3" t="s">
         <v>113</v>
       </c>
@@ -3924,7 +4720,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>118</v>
       </c>
@@ -3946,7 +4742,7 @@
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="2:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B4" s="11" t="s">
         <v>120</v>
       </c>
@@ -3978,7 +4774,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="2:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B5" s="11" t="s">
         <v>123</v>
       </c>
@@ -4010,7 +4806,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="2:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B6" s="11" t="s">
         <v>126</v>
       </c>
@@ -4042,7 +4838,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="2:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B7" s="11" t="s">
         <v>129</v>
       </c>
@@ -4074,7 +4870,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="2:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B8" s="11" t="s">
         <v>132</v>
       </c>
@@ -4106,7 +4902,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="2:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B9" s="11" t="s">
         <v>135</v>
       </c>
@@ -4138,7 +4934,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="2:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B10" s="11" t="s">
         <v>138</v>
       </c>
@@ -4170,7 +4966,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="2:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B11" s="11" t="s">
         <v>141</v>
       </c>
@@ -4202,7 +4998,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="2:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B12" s="11" t="s">
         <v>144</v>
       </c>
@@ -4234,7 +5030,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="2:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B13" s="11" t="s">
         <v>147</v>
       </c>
@@ -4266,7 +5062,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="2:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B14" s="11" t="s">
         <v>150</v>
       </c>
@@ -4298,7 +5094,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="2:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B15" s="28" t="s">
         <v>153</v>
       </c>
@@ -4330,7 +5126,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D17" s="43"/>
     </row>
   </sheetData>
@@ -4347,20 +5143,20 @@
       <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="60.7109375" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" customWidth="1"/>
-    <col min="4" max="4" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.28515625" customWidth="1"/>
-    <col min="10" max="10" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="60.6640625" customWidth="1"/>
+    <col min="3" max="3" width="18.5546875" customWidth="1"/>
+    <col min="4" max="4" width="31.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.33203125" customWidth="1"/>
+    <col min="10" max="10" width="29.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C2" s="25" t="s">
         <v>157</v>
       </c>
@@ -4386,7 +5182,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
       <c r="E3" s="30"/>
@@ -4396,7 +5192,7 @@
       <c r="I3" s="30"/>
       <c r="J3" s="30"/>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C4" s="25"/>
       <c r="D4" s="25"/>
       <c r="E4" s="25"/>
@@ -4406,7 +5202,7 @@
       <c r="I4" s="25"/>
       <c r="J4" s="25"/>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C5" s="25" t="s">
         <v>104</v>
       </c>
@@ -4432,7 +5228,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>118</v>
       </c>
@@ -4445,7 +5241,7 @@
       <c r="I6" s="23"/>
       <c r="J6" s="23"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B7" s="11" t="s">
         <v>120</v>
       </c>
@@ -4458,7 +5254,7 @@
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B8" s="11" t="s">
         <v>123</v>
       </c>
@@ -4471,7 +5267,7 @@
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B9" s="11" t="s">
         <v>126</v>
       </c>
@@ -4484,7 +5280,7 @@
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B10" s="11" t="s">
         <v>129</v>
       </c>
@@ -4497,7 +5293,7 @@
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B11" s="11" t="s">
         <v>132</v>
       </c>
@@ -4510,7 +5306,7 @@
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B12" s="11" t="s">
         <v>135</v>
       </c>
@@ -4523,7 +5319,7 @@
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B13" s="11" t="s">
         <v>138</v>
       </c>
@@ -4536,7 +5332,7 @@
       <c r="I13" s="29"/>
       <c r="J13" s="29"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B14" s="11" t="s">
         <v>141</v>
       </c>
@@ -4549,7 +5345,7 @@
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B15" s="11" t="s">
         <v>144</v>
       </c>
@@ -4562,7 +5358,7 @@
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B16" s="11" t="s">
         <v>147</v>
       </c>
@@ -4575,7 +5371,7 @@
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B17" s="11" t="s">
         <v>150</v>
       </c>
@@ -4588,7 +5384,7 @@
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B18" s="28" t="s">
         <v>153</v>
       </c>
@@ -4601,7 +5397,7 @@
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
         <v>106</v>
       </c>
@@ -4614,7 +5410,7 @@
       <c r="I19" s="9"/>
       <c r="J19" s="9"/>
     </row>
-    <row r="20" spans="2:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B20" s="11" t="s">
         <v>107</v>
       </c>
@@ -4645,22 +5441,22 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31" style="42" customWidth="1"/>
     <col min="4" max="4" width="47" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" customWidth="1"/>
-    <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.85546875" customWidth="1"/>
+    <col min="7" max="7" width="15.88671875" customWidth="1"/>
+    <col min="8" max="8" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.88671875" customWidth="1"/>
     <col min="10" max="10" width="19" customWidth="1"/>
-    <col min="11" max="11" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.28515625" customWidth="1"/>
+    <col min="11" max="11" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B2" s="33"/>
       <c r="C2" s="40"/>
       <c r="D2" s="35"/>
@@ -4688,7 +5484,7 @@
       </c>
       <c r="M2" s="33"/>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B3" s="33"/>
       <c r="C3" s="40"/>
       <c r="D3" s="35"/>
@@ -4716,7 +5512,7 @@
       </c>
       <c r="M3" s="33"/>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B4" s="33"/>
       <c r="C4" s="40"/>
       <c r="D4" s="35"/>
@@ -4730,7 +5526,7 @@
       <c r="L4" s="34"/>
       <c r="M4" s="33"/>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B5" s="34" t="s">
         <v>177</v>
       </c>
@@ -4752,7 +5548,7 @@
       <c r="L5" s="34"/>
       <c r="M5" s="33"/>
     </row>
-    <row r="6" spans="2:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B6" s="17" t="s">
         <v>178</v>
       </c>
@@ -4788,7 +5584,7 @@
       </c>
       <c r="M6" s="33"/>
     </row>
-    <row r="7" spans="2:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B7" s="17" t="s">
         <v>182</v>
       </c>
@@ -4824,7 +5620,7 @@
       </c>
       <c r="M7" s="33"/>
     </row>
-    <row r="8" spans="2:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B8" s="17" t="s">
         <v>185</v>
       </c>
@@ -4860,7 +5656,7 @@
       </c>
       <c r="M8" s="33"/>
     </row>
-    <row r="9" spans="2:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B9" s="17" t="s">
         <v>169</v>
       </c>
@@ -4896,7 +5692,7 @@
       </c>
       <c r="M9" s="33"/>
     </row>
-    <row r="10" spans="2:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B10" s="17" t="s">
         <v>190</v>
       </c>
@@ -4932,7 +5728,7 @@
       </c>
       <c r="M10" s="33"/>
     </row>
-    <row r="11" spans="2:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B11" s="17" t="s">
         <v>193</v>
       </c>
@@ -4968,7 +5764,7 @@
       </c>
       <c r="M11" s="33"/>
     </row>
-    <row r="12" spans="2:13" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:13" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="17" t="s">
         <v>196</v>
       </c>
@@ -5004,7 +5800,7 @@
       </c>
       <c r="M12" s="33"/>
     </row>
-    <row r="13" spans="2:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B13" s="17" t="s">
         <v>200</v>
       </c>
@@ -5040,7 +5836,7 @@
       </c>
       <c r="M13" s="33"/>
     </row>
-    <row r="14" spans="2:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B14" s="17" t="s">
         <v>203</v>
       </c>
@@ -5076,7 +5872,7 @@
       </c>
       <c r="M14" s="33"/>
     </row>
-    <row r="15" spans="2:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B15" s="17" t="s">
         <v>207</v>
       </c>
@@ -5112,7 +5908,7 @@
       </c>
       <c r="M15" s="33"/>
     </row>
-    <row r="16" spans="2:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B16" s="17" t="s">
         <v>211</v>
       </c>
@@ -5148,7 +5944,7 @@
       </c>
       <c r="M16" s="33"/>
     </row>
-    <row r="17" spans="2:13" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:13" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="17" t="s">
         <v>214</v>
       </c>
@@ -5184,7 +5980,7 @@
       </c>
       <c r="M17" s="33"/>
     </row>
-    <row r="18" spans="2:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B18" s="17" t="s">
         <v>217</v>
       </c>
@@ -5220,7 +6016,7 @@
       </c>
       <c r="M18" s="33"/>
     </row>
-    <row r="19" spans="2:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B19" s="37" t="s">
         <v>220</v>
       </c>
@@ -5270,19 +6066,19 @@
       <selection activeCell="P1" sqref="P1:P1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" customWidth="1"/>
-    <col min="5" max="5" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15.88671875" customWidth="1"/>
+    <col min="5" max="5" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.88671875" customWidth="1"/>
     <col min="7" max="7" width="19" customWidth="1"/>
-    <col min="8" max="8" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="15" width="20.28515625" customWidth="1"/>
+    <col min="8" max="8" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="15" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" s="44" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:16" s="44" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C2" s="36" t="s">
         <v>223</v>
       </c>
@@ -5323,7 +6119,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B3" s="33"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -5340,7 +6136,7 @@
       <c r="O3" s="5"/>
       <c r="P3" s="33"/>
     </row>
-    <row r="4" spans="2:16" s="46" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:16" s="46" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C4" s="25" t="s">
         <v>168</v>
       </c>
@@ -5381,7 +6177,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B5" s="34" t="s">
         <v>118</v>
       </c>
@@ -5400,7 +6196,7 @@
       <c r="O5" s="34"/>
       <c r="P5" s="33"/>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B6" s="17" t="s">
         <v>178</v>
       </c>
@@ -5423,7 +6219,7 @@
       <c r="O6" s="4"/>
       <c r="P6" s="33"/>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B7" s="17" t="s">
         <v>182</v>
       </c>
@@ -5446,7 +6242,7 @@
       <c r="O7" s="4"/>
       <c r="P7" s="33"/>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B8" s="17" t="s">
         <v>185</v>
       </c>
@@ -5469,7 +6265,7 @@
       <c r="O8" s="4"/>
       <c r="P8" s="33"/>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B9" s="17" t="s">
         <v>169</v>
       </c>
@@ -5492,7 +6288,7 @@
       <c r="O9" s="4"/>
       <c r="P9" s="33"/>
     </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B10" s="17" t="s">
         <v>190</v>
       </c>
@@ -5515,7 +6311,7 @@
       <c r="O10" s="4"/>
       <c r="P10" s="33"/>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B11" s="17" t="s">
         <v>193</v>
       </c>
@@ -5538,7 +6334,7 @@
       <c r="O11" s="4"/>
       <c r="P11" s="33"/>
     </row>
-    <row r="12" spans="2:16" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:16" ht="41.4" x14ac:dyDescent="0.3">
       <c r="B12" s="17" t="s">
         <v>196</v>
       </c>
@@ -5561,7 +6357,7 @@
       <c r="O12" s="10"/>
       <c r="P12" s="33"/>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B13" s="17" t="s">
         <v>200</v>
       </c>
@@ -5584,7 +6380,7 @@
       <c r="O13" s="4"/>
       <c r="P13" s="33"/>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B14" s="17" t="s">
         <v>203</v>
       </c>
@@ -5607,7 +6403,7 @@
       <c r="O14" s="10"/>
       <c r="P14" s="33"/>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B15" s="17" t="s">
         <v>207</v>
       </c>
@@ -5630,7 +6426,7 @@
       <c r="O15" s="4"/>
       <c r="P15" s="33"/>
     </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B16" s="17" t="s">
         <v>211</v>
       </c>
@@ -5653,7 +6449,7 @@
       <c r="O16" s="4"/>
       <c r="P16" s="33"/>
     </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B17" s="17" t="s">
         <v>214</v>
       </c>
@@ -5676,7 +6472,7 @@
       <c r="O17" s="4"/>
       <c r="P17" s="33"/>
     </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B18" s="17" t="s">
         <v>217</v>
       </c>
@@ -5699,7 +6495,7 @@
       <c r="O18" s="4"/>
       <c r="P18" s="33"/>
     </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B19" s="37" t="s">
         <v>220</v>
       </c>
@@ -5722,22 +6518,22 @@
       <c r="O19" s="4"/>
       <c r="P19" s="33"/>
     </row>
-    <row r="20" spans="2:16" ht="135" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:16" ht="115.2" x14ac:dyDescent="0.3">
       <c r="K20" s="48" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="21" spans="2:16" ht="90" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:16" ht="86.4" x14ac:dyDescent="0.3">
       <c r="K21" s="49" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="22" spans="2:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:16" ht="43.2" x14ac:dyDescent="0.3">
       <c r="K22" s="50" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="23" spans="2:16" ht="75" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:16" ht="72" x14ac:dyDescent="0.3">
       <c r="K23" s="50" t="s">
         <v>244</v>
       </c>
@@ -5753,19 +6549,1094 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E11F00D1-5894-4EDF-B883-7004CBBD10B4}">
+  <dimension ref="B2:L32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="28.77734375" style="68" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.88671875" style="14" customWidth="1"/>
+    <col min="4" max="4" width="38.21875" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" customWidth="1"/>
+    <col min="6" max="6" width="31.44140625" customWidth="1"/>
+    <col min="7" max="7" width="28.6640625" customWidth="1"/>
+    <col min="8" max="8" width="36.5546875" customWidth="1"/>
+    <col min="9" max="10" width="30.21875" customWidth="1"/>
+    <col min="11" max="11" width="34.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="31.21875" style="69" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:12" s="14" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B2" s="15" t="s">
+        <v>245</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="36" t="s">
+        <v>246</v>
+      </c>
+      <c r="G2" s="36" t="s">
+        <v>247</v>
+      </c>
+      <c r="H2" s="36" t="s">
+        <v>248</v>
+      </c>
+      <c r="I2" s="36" t="s">
+        <v>249</v>
+      </c>
+      <c r="J2" s="36" t="s">
+        <v>250</v>
+      </c>
+      <c r="K2" s="36" t="s">
+        <v>251</v>
+      </c>
+      <c r="L2" s="36" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B3" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="52" t="s">
+        <v>254</v>
+      </c>
+      <c r="G3" s="53" t="s">
+        <v>255</v>
+      </c>
+      <c r="H3" s="52" t="s">
+        <v>256</v>
+      </c>
+      <c r="I3" s="52" t="s">
+        <v>257</v>
+      </c>
+      <c r="J3" s="52" t="s">
+        <v>258</v>
+      </c>
+      <c r="K3" s="52" t="s">
+        <v>259</v>
+      </c>
+      <c r="L3" s="54" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="B4" s="55" t="s">
+        <v>261</v>
+      </c>
+      <c r="C4" s="51"/>
+      <c r="D4" s="56" t="s">
+        <v>262</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>263</v>
+      </c>
+      <c r="G4" s="18" t="s">
+        <v>264</v>
+      </c>
+      <c r="H4" s="40" t="s">
+        <v>265</v>
+      </c>
+      <c r="I4" s="57" t="s">
+        <v>266</v>
+      </c>
+      <c r="J4" s="57" t="s">
+        <v>267</v>
+      </c>
+      <c r="K4" s="18" t="s">
+        <v>268</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B5" s="55" t="s">
+        <v>270</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>271</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>273</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>273</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>273</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>273</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>273</v>
+      </c>
+      <c r="K5" s="10" t="s">
+        <v>273</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="55" t="s">
+        <v>275</v>
+      </c>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K6" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="L6" s="4"/>
+    </row>
+    <row r="7" spans="2:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B7" s="55" t="s">
+        <v>278</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>279</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B8" s="55" t="s">
+        <v>281</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>282</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>283</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L8" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="B9" s="55" t="s">
+        <v>284</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>285</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>286</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>287</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L9" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="B10" s="17" t="s">
+        <v>288</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>289</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="J10" s="10" t="s">
+        <v>294</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L10" s="10" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B11" s="55" t="s">
+        <v>296</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>297</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>298</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>299</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L11" s="58" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B12" s="55" t="s">
+        <v>300</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>301</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>302</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L12" s="58" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B13" s="55" t="s">
+        <v>303</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>304</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>305</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L13" s="59" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B14" s="55" t="s">
+        <v>306</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>307</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>308</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L14" s="58" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B15" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>310</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>311</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L15" s="59" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B16" s="17" t="s">
+        <v>312</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>313</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>314</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="I16" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="J16" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="K16" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="L16" s="59" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" ht="216" x14ac:dyDescent="0.3">
+      <c r="B17" s="17" t="s">
+        <v>315</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>316</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>314</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="60" t="s">
+        <v>317</v>
+      </c>
+      <c r="G17" s="61" t="s">
+        <v>318</v>
+      </c>
+      <c r="H17" s="61" t="s">
+        <v>319</v>
+      </c>
+      <c r="I17" s="61" t="s">
+        <v>320</v>
+      </c>
+      <c r="J17" s="61" t="s">
+        <v>321</v>
+      </c>
+      <c r="K17" s="61" t="s">
+        <v>322</v>
+      </c>
+      <c r="L17" s="62" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="B18" s="18" t="s">
+        <v>324</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>325</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>326</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F18" s="61" t="s">
+        <v>327</v>
+      </c>
+      <c r="G18" s="61" t="s">
+        <v>328</v>
+      </c>
+      <c r="H18" s="61" t="s">
+        <v>329</v>
+      </c>
+      <c r="I18" s="61" t="s">
+        <v>330</v>
+      </c>
+      <c r="J18" s="61" t="s">
+        <v>329</v>
+      </c>
+      <c r="K18" s="61" t="s">
+        <v>331</v>
+      </c>
+      <c r="L18" s="62" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" ht="72" x14ac:dyDescent="0.3">
+      <c r="B19" s="13" t="s">
+        <v>333</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>334</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>335</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J19" s="63" t="s">
+        <v>336</v>
+      </c>
+      <c r="K19" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L19" s="59" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B20" s="11" t="s">
+        <v>337</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>338</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>339</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>340</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H20" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="I20" s="10" t="s">
+        <v>342</v>
+      </c>
+      <c r="J20" s="64" t="s">
+        <v>343</v>
+      </c>
+      <c r="K20" s="64" t="s">
+        <v>344</v>
+      </c>
+      <c r="L20" s="59" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" ht="72" x14ac:dyDescent="0.3">
+      <c r="B21" s="11" t="s">
+        <v>346</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>347</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>348</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" s="65" t="s">
+        <v>349</v>
+      </c>
+      <c r="G21" s="65" t="s">
+        <v>350</v>
+      </c>
+      <c r="H21" s="65" t="s">
+        <v>351</v>
+      </c>
+      <c r="I21" s="65" t="s">
+        <v>352</v>
+      </c>
+      <c r="J21" s="66" t="s">
+        <v>353</v>
+      </c>
+      <c r="K21" s="67" t="s">
+        <v>354</v>
+      </c>
+      <c r="L21" s="62" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B22" s="17" t="s">
+        <v>356</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>357</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>358</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>359</v>
+      </c>
+      <c r="G22" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K22" s="4" t="s">
+        <v>361</v>
+      </c>
+      <c r="L22" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B23" s="11" t="s">
+        <v>362</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>363</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>364</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>365</v>
+      </c>
+      <c r="G23" s="64" t="s">
+        <v>366</v>
+      </c>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4" t="s">
+        <v>367</v>
+      </c>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B24" s="11" t="s">
+        <v>368</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>369</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>370</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>373</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>373</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="K24" s="63" t="s">
+        <v>374</v>
+      </c>
+      <c r="L24" s="59" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="B25" s="13" t="s">
+        <v>376</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>377</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>378</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G25" s="10" t="s">
+        <v>379</v>
+      </c>
+      <c r="H25" s="4"/>
+      <c r="I25" s="64" t="s">
+        <v>380</v>
+      </c>
+      <c r="J25" s="64" t="s">
+        <v>381</v>
+      </c>
+      <c r="K25" s="63" t="s">
+        <v>382</v>
+      </c>
+      <c r="L25" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B26" s="11" t="s">
+        <v>383</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>384</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>385</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="K26" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L26" s="59" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B27" s="11" t="s">
+        <v>388</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>389</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>390</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>391</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="I27" s="64" t="s">
+        <v>394</v>
+      </c>
+      <c r="J27" s="4" t="s">
+        <v>395</v>
+      </c>
+      <c r="K27" s="4" t="s">
+        <v>395</v>
+      </c>
+      <c r="L27" s="4" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="B28" s="11" t="s">
+        <v>397</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>399</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F28" s="61" t="s">
+        <v>400</v>
+      </c>
+      <c r="G28" s="10" t="s">
+        <v>401</v>
+      </c>
+      <c r="H28" s="10" t="s">
+        <v>402</v>
+      </c>
+      <c r="I28" s="10" t="s">
+        <v>403</v>
+      </c>
+      <c r="J28" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K28" s="63" t="s">
+        <v>404</v>
+      </c>
+      <c r="L28" s="10" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="B29" s="17" t="s">
+        <v>406</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>407</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>408</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F29" s="61" t="s">
+        <v>409</v>
+      </c>
+      <c r="G29" s="61" t="s">
+        <v>410</v>
+      </c>
+      <c r="H29" s="61" t="s">
+        <v>411</v>
+      </c>
+      <c r="I29" s="61" t="s">
+        <v>412</v>
+      </c>
+      <c r="J29" s="61" t="s">
+        <v>413</v>
+      </c>
+      <c r="K29" s="61" t="s">
+        <v>414</v>
+      </c>
+      <c r="L29" s="61" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B30" s="11" t="s">
+        <v>416</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>417</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>418</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I30" s="10" t="s">
+        <v>419</v>
+      </c>
+      <c r="J30" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K30" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="L30" s="10" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="B31" s="11" t="s">
+        <v>422</v>
+      </c>
+      <c r="C31" s="51"/>
+      <c r="D31" s="51"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="18" t="s">
+        <v>423</v>
+      </c>
+      <c r="I31" s="4"/>
+      <c r="J31" s="18" t="s">
+        <v>424</v>
+      </c>
+      <c r="K31" s="61" t="s">
+        <v>425</v>
+      </c>
+      <c r="L31" s="58"/>
+    </row>
+    <row r="32" spans="2:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B32" s="11" t="s">
+        <v>426</v>
+      </c>
+      <c r="C32" s="51"/>
+      <c r="D32" s="13" t="s">
+        <v>427</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F32" s="64" t="s">
+        <v>428</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>429</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>429</v>
+      </c>
+      <c r="I32" s="4" t="s">
+        <v>429</v>
+      </c>
+      <c r="J32" s="4" t="s">
+        <v>429</v>
+      </c>
+      <c r="K32" s="4" t="s">
+        <v>430</v>
+      </c>
+      <c r="L32" s="10" t="s">
+        <v>430</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F3" r:id="rId1" xr:uid="{8BE67516-8BC9-4B31-97EB-B9CCF15D8E23}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{DBF6232F-3EB0-45B2-A888-5587B47340C1}"/>
+    <hyperlink ref="K3" r:id="rId3" xr:uid="{8F8E0DDB-244C-4A05-A569-20AB947DBB14}"/>
+    <hyperlink ref="I3" r:id="rId4" xr:uid="{93596F5F-9DF7-4097-98FD-306938A4AC95}"/>
+    <hyperlink ref="H3" r:id="rId5" xr:uid="{6BD62EFC-A953-492A-987D-41348BEA0602}"/>
+    <hyperlink ref="J3" r:id="rId6" xr:uid="{776565E1-78D4-4F66-BCC7-723FFA35DE82}"/>
+    <hyperlink ref="L3" r:id="rId7" xr:uid="{D7ADECC0-0F30-4B67-8AB4-CAF7400EFC03}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5972,14 +7843,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FBD369E-6A68-4C96-8DEA-0EC45C5264AD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{32AD9959-A697-4819-834E-1AB73008AA4B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -5992,6 +7855,14 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="680bcac6-b14c-4c2b-a58b-c019311aeaad"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FBD369E-6A68-4C96-8DEA-0EC45C5264AD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Adding Content Management System content
</commit_message>
<xml_diff>
--- a/documents/common-component-matrix.xlsx
+++ b/documents/common-component-matrix.xlsx
@@ -1,24 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\DFE\Top15\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\github\architecture\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AA99E81D-BD3E-4D7C-9BEE-B53C5EF7943F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B1EE814-4381-496C-8184-565EDF3AA24F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9060" yWindow="1740" windowWidth="25170" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25320" yWindow="-120" windowWidth="25440" windowHeight="15390" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping Applications" sheetId="1" r:id="rId1"/>
-    <sheet name="Mapping Services" sheetId="4" r:id="rId2"/>
-    <sheet name="Postcode Applications" sheetId="5" r:id="rId3"/>
-    <sheet name="Postcode Services" sheetId="6" r:id="rId4"/>
-    <sheet name="Notification Application" sheetId="7" r:id="rId5"/>
-    <sheet name="Notification Services" sheetId="8" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="9" r:id="rId2"/>
+    <sheet name="Mapping Services" sheetId="4" r:id="rId3"/>
+    <sheet name="Postcode Applications" sheetId="5" r:id="rId4"/>
+    <sheet name="Postcode Services" sheetId="6" r:id="rId5"/>
+    <sheet name="Notification Application" sheetId="7" r:id="rId6"/>
+    <sheet name="Notification Services" sheetId="8" r:id="rId7"/>
+    <sheet name="CMS Applications" sheetId="11" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -1263,7 +1265,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="991" uniqueCount="431">
   <si>
     <t>Azure Maps</t>
   </si>
@@ -2051,12 +2053,742 @@
   <si>
     <t>https://dfedigital.atlassian.net/wiki/spaces/TSTL/pages/1223458929/What+we+use+and+defaults</t>
   </si>
+  <si>
+    <t>Feature</t>
+  </si>
+  <si>
+    <t>Contentful</t>
+  </si>
+  <si>
+    <t>Contentstack</t>
+  </si>
+  <si>
+    <t>Kontent</t>
+  </si>
+  <si>
+    <t>Prismic</t>
+  </si>
+  <si>
+    <t>Cosmic JS</t>
+  </si>
+  <si>
+    <t>Sitefinity</t>
+  </si>
+  <si>
+    <t>OrchardCore</t>
+  </si>
+  <si>
+    <t>Weblink</t>
+  </si>
+  <si>
+    <t>https://www.contentful.com/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.contentstack.com/ </t>
+  </si>
+  <si>
+    <t>https://kontent.ai/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://prismic.io/ </t>
+  </si>
+  <si>
+    <t>https://www.cosmicjs.com/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.progress.com/sitefinity-cms </t>
+  </si>
+  <si>
+    <t>http://www.orchardcore.net/</t>
+  </si>
+  <si>
+    <t>Licence Type/Pricing Structure</t>
+  </si>
+  <si>
+    <t>Dependent on usecases, specific requirements (inc. specialist language content) and size of service</t>
+  </si>
+  <si>
+    <t>•	On-demand = Pay for the space only
+•	Micro = €420/year (1 master and 1 sandbox environment, 1 role, 2 locales, 24 content types, 5,000 records)
+•	Small = €2,028/year (1 master and 2 sandbox environment, 2 role, 4 locales, 24 content types, 10,000 records)
+•	Medium = €5,268/year (1 master and 3 sandbox environment, 2 role, 7 locales, 48 content types, 25,000 records)
+•	Large = €9,468/year (1 master and 5 sandbox environment, 4 role, 10 locales, 48 content types, 50,000 records, plus GraphQL API)
+•	Enterprise = Pay for the platform + SLA + space
+•	Professional = €24,000+/year (+ space and SLA costs) - custom roles, SSO, full webhook functionality, scheduled publishing
+•	Scale = €90,000+/year (+ space and SLA costs)
+•	High availability = €225,000+/year (+ space and SLA costs)</t>
+  </si>
+  <si>
+    <t>•Business = $3,500/month
+-10 Users
+- 1 Property
+- Content Types
+- Digital Assets Management
+- Rich Text Editor
+- Multiple Environments
+- Modular Blocks (Page Builder)
+- Custom Fields
+•Enterprise = Starts at $10,000/month (requires quotation) and onboarding fee required for first year
+- 10+ Users
+- 3+ Properties
+- Workflows
+- Grouped Releases
+- Bulk Operations
+- Experience Extensions (Integrations)
+- Dashboard
+- Analytics</t>
+  </si>
+  <si>
+    <t>•Starter = Free
+- 3 Users ($10/month per extra user. Max 20 users)
+- Unlimited projects (but without ability to clone)
+- 5,000 Content items
+- 2 Languages
+•Business = $999/month
+- 15 Users ($10/month per extra user. Max 30 users)
+- Unlimited projects
+- 25,000 Content items
+- 10 Languages
+- 1 predefined role + 2 Custom roles
+•Enterprise = Starts at $1,499/month (requires quotation)
+- Custom number of Users
+- Unlimited projects
+- More Content items
+- More Languages
+- More Custom roles</t>
+  </si>
+  <si>
+    <t>•Free and Starter are the cheapest tiers
+•Small = $20/month OR $15/month for annual contract
+- 7 Users
+- Basic Support
+- Core features
+•Professional - Medium = $125/month OR $100/month for annual contract
+- 25 Users
+- SLA (99,5% API Uptime), Basic Support
+- User roles, publication workflow &amp; collaboration features
+•Professional - Platinum = $575/month OR $500/month for annual contract
+- Unlimited users
+- SLA (99,5% API Uptime), Priority Support
+- User roles, publication workflow &amp; collaboration features
+•Enterprise = Starts at $24,000/year (requires quotation)
+- Includes three environments (development, staging, production)
+- SLA (99.95% API Uptime)
+- Daily backups &amp; snapshots
+- SSO and MFA</t>
+  </si>
+  <si>
+    <t>•	Personal Plan provides a free option
+•	Starter = $99/month (10% off for annual)
+- Single Bucket
+- 5 team members
+- 25,000 API requests
+- 10,000 files / 3GB media storage
+•	Pro = $299/month (10% off for annual)
+- Single Bucket
+- 10 team members
+- 150,000 API requests
+- 50,000 files / 15GB media storage
+•	Business = $799/month (10% off for annual)
+- Single Bucket
+- 30 team members
+- 500,000 API requests
+- 100,000 files / 50GB media storage
+•	Enterprise = requires quotation
+- Dedicated Infrastructure
+- Single Sign-on
+- 24/7 Support
+- SLA
+- Migration Support
+- All add-ons included
+- Company workspace</t>
+  </si>
+  <si>
+    <t>•	Professional Edition = Starts at $15,000/year (requires quotation)
+- 1 production domain or server
+- 10 concurrent users
+- Web Content Management
+- Developer Productivity Tools
+•	Online Marketing Edition = Starts at $30,000+/year (requires quotation)
+- 1 production domain
+- 15 concurrent users
+- Web Content Management
+- Developer Productivity Tools
+- Marketing and CRM connectors
+- Content personalisation
+•	Enterprise Edition = Starts at $50,000/year (requires quotation)
+- Unlimited concurrent users
+- Web Content Management
+- Developer Productivity Tools
+- All connectors
+- Content personalisation
+- Site sync between environments
+- Translations management
+- System audit trail</t>
+  </si>
+  <si>
+    <t>Opensource</t>
+  </si>
+  <si>
+    <t>Service Type</t>
+  </si>
+  <si>
+    <t>Cloud based or on Prem</t>
+  </si>
+  <si>
+    <t>As a product owner I want a CMS service to develop content so that I can publish digital content online.</t>
+  </si>
+  <si>
+    <t>SaaS</t>
+  </si>
+  <si>
+    <t>PaaS</t>
+  </si>
+  <si>
+    <t>Compatible with Ruby on Rails</t>
+  </si>
+  <si>
+    <t>As a product owner I want….</t>
+  </si>
+  <si>
+    <t>N 
+(.Net platform)</t>
+  </si>
+  <si>
+    <t>Restful API</t>
+  </si>
+  <si>
+    <t>Allows it to communicate with other services and components, using best practice protocols</t>
+  </si>
+  <si>
+    <t>As a product owner I want the CMS to be interoperable with other component and services so that the platform is extensible.</t>
+  </si>
+  <si>
+    <t>Graph QL</t>
+  </si>
+  <si>
+    <t>Query language for APIs</t>
+  </si>
+  <si>
+    <t>As a product owner I want be able to query the data held within the CMS so that I can search for specific information.</t>
+  </si>
+  <si>
+    <t>Supports webhooks</t>
+  </si>
+  <si>
+    <t>Provide real-time event driven information</t>
+  </si>
+  <si>
+    <t>As a product owner I want to use webhooks for my app or platform so that I can provide a real-time without developing an AP.</t>
+  </si>
+  <si>
+    <t>Y
+- Webhooks supported but functionality is limited below Enterprise level (e.g. not possible to trigger a webhook off certain "event" types). Templates and static webhook IPs provided in Enterprise version.</t>
+  </si>
+  <si>
+    <t>Integrations</t>
+  </si>
+  <si>
+    <t>Ability to interface and connect with other platforms and services</t>
+  </si>
+  <si>
+    <t>API</t>
+  </si>
+  <si>
+    <t>API
+- Integrates with martech technologies such as Marketo, Salesforce, Google Analytics, SEMrush, Brightcove, Watson, etc.
+- Integrations with Google Docs and Slack are being developed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+- Integration with task management tools such as Trello, Jira and Asana in the roadmap
+- Delivery API not exposed in free Starter version.</t>
+  </si>
+  <si>
+    <t>API
+- Integrations with Slack being discussed but still in the roadmap</t>
+  </si>
+  <si>
+    <t>API
+-Integration with a number of web services including Slack, GitHub, Google Analytics</t>
+  </si>
+  <si>
+    <t>Integrated with NEO for GraghQL interface/ Sparql (WC3 standard)</t>
+  </si>
+  <si>
+    <t>Notifications</t>
+  </si>
+  <si>
+    <t>Ability to send and receive messages in different applications</t>
+  </si>
+  <si>
+    <t>As a product owner I want to be able to send messages from the CMS so other platforms or service so that I can communicate with users.</t>
+  </si>
+  <si>
+    <t>Y
+- Notifications work in Slack as well as email</t>
+  </si>
+  <si>
+    <t>Content Previewing</t>
+  </si>
+  <si>
+    <t>To be able to preview content before it is published online</t>
+  </si>
+  <si>
+    <t>As a product owner I want I want to view my content before it is published online so that I can validate it is correct.</t>
+  </si>
+  <si>
+    <t>Rich Text Format Editor</t>
+  </si>
+  <si>
+    <t>Text formatting options</t>
+  </si>
+  <si>
+    <t>As a product owner I want to be able to format the text so that it is accessible for the audience.</t>
+  </si>
+  <si>
+    <t>Version History</t>
+  </si>
+  <si>
+    <t>To be able number and keep a log of historic releases</t>
+  </si>
+  <si>
+    <t>As a product owner I want to be able to view the history of published changes so that I have a record of past versions.</t>
+  </si>
+  <si>
+    <t>Scheduled Publishing</t>
+  </si>
+  <si>
+    <t>Ability to set the time content is to be published</t>
+  </si>
+  <si>
+    <t>As a product owner I want develop and release content at a plannned time so that content is published at the scheduled time.</t>
+  </si>
+  <si>
+    <t>Publishing Approval Workflow</t>
+  </si>
+  <si>
+    <t>Automated approval sign off for content before it is published</t>
+  </si>
+  <si>
+    <t>As a product owner I want changes to content to go through a business approval process so that the necessary checks are in place before publishing.</t>
+  </si>
+  <si>
+    <t>Workflow Tools</t>
+  </si>
+  <si>
+    <t>Ability to define processes and workflows to create, approve and publish content</t>
+  </si>
+  <si>
+    <t>- Content approval Workflows
+- Notifications only available in Enterprise plans
+- Custom roles only available in Enterprise plans
+- Content publishing and expiry scheduling only available in Enterprise plans
+- Content versioning and revision history for all plans</t>
+  </si>
+  <si>
+    <t>- Content publishing and expiry scheduling for all plans
+- Versioning and rollback
+- Built in approval workflows only available in Enterprise version
+- Ability to use webhooks for notifications limited below Enterprise
+- Grouped releases only available in Enterprise version</t>
+  </si>
+  <si>
+    <t>- Request review and approve content workflow (excluding free version)
+- Ability to leave comments and suggest changes for approval (excluding free version)
+- Built in notifications tool (email and Slack)
+- No limit on how webhooks are used for notifications
+- Revision history
+- Content publishing and expiry scheduling (excluding free version)
+- Dashboard view of assignments
+- Calendar view to see upcoming publishing or content expiry dates</t>
+  </si>
+  <si>
+    <t>- User roles limited to three (admin, publisher, writer) with no custom roles
+- Publishing workflow tool available in all plans
+- No limits on how webhooks are used for notifications
+- Release scheduling and bulk publishing for all plans
+- Full revision history</t>
+  </si>
+  <si>
+    <t>- Ability to build content publishing workflow for all plans
+- Zapier used for notifications
+- Scheduled publishing and expiry for all plans
+- Revision history for all plans</t>
+  </si>
+  <si>
+    <t>- Approval workflow tools and user permissions
+- Built in email notification tool
+- No limits on how webhooks are used for notifications
+- Content Publication &amp; Expiration Scheduling for all plans</t>
+  </si>
+  <si>
+    <t>Can develop and edit workflows</t>
+  </si>
+  <si>
+    <t>Multimedia Capability</t>
+  </si>
+  <si>
+    <t>Ability to Support media files such as images, videos, sound files etc</t>
+  </si>
+  <si>
+    <t>As a product owner I want to publish multimedia content so that I can give a rich user experience to the user.</t>
+  </si>
+  <si>
+    <t>- Wide variety of content modelling options- content types include text, dates, rich text, media (images, docs etc.), location, references to other content, arrays and even JSON for data.</t>
+  </si>
+  <si>
+    <t>- Supports all media files such as image link, video link, GIFs etc.
+- Maximum size of a single asset file is 700 MB (this can be restricted further using validation rules).</t>
+  </si>
+  <si>
+    <t>- Asset library supports a range of media types</t>
+  </si>
+  <si>
+    <t>- Every repository on Prismic has its own media library, which supports a range of file types including images, sounds files, videos, pdfs and more.
+- Max image size is 10Mb and max for any other file type is 100Mb
+- Imgix API used to make builds with images easier</t>
+  </si>
+  <si>
+    <t>- Supports a wide variety of media types including video.</t>
+  </si>
+  <si>
+    <t>No image manipulaton/ can use CDL</t>
+  </si>
+  <si>
+    <t>Secure Hosting</t>
+  </si>
+  <si>
+    <t>Hosting that is encrypted at rest and intransit and accessed securley (physical and digital). And hosted in a secure location.</t>
+  </si>
+  <si>
+    <t>As a product owner I want a secure service so that I can deliver content that is security compliant.</t>
+  </si>
+  <si>
+    <t>- Use AWS hosting</t>
+  </si>
+  <si>
+    <t>Multifactor Authentication</t>
+  </si>
+  <si>
+    <t>Enhanced authentication capability</t>
+  </si>
+  <si>
+    <t>As a product owner I want to keep access to the CMS platform secure so that only authorised user can access the platform.</t>
+  </si>
+  <si>
+    <t>Y
+- 2FA is an option even for the free tier but it is not enforced</t>
+  </si>
+  <si>
+    <t>Y
+For Enterprise Plans</t>
+  </si>
+  <si>
+    <t>Y
+Two factor authentication for Enterprise plans</t>
+  </si>
+  <si>
+    <t>- Two-factor authentication included for all plans.</t>
+  </si>
+  <si>
+    <t>- Windows and other authenticator options</t>
+  </si>
+  <si>
+    <t>Requires development and integration into identity provider</t>
+  </si>
+  <si>
+    <t>Security Certification</t>
+  </si>
+  <si>
+    <t>Provider is compliant with required standards</t>
+  </si>
+  <si>
+    <t>As a product owner I want the assurance that the CMS platform provider can demonstrate security compliance so that I know the platform will be secure to deliver my service.</t>
+  </si>
+  <si>
+    <t>Y 
+(ISO 27001:2013 compliant and ISO 27001 compliant data centres)</t>
+  </si>
+  <si>
+    <t>Y
+- SOC 2 Type II certification
+- ISO 27001 Compliant Data Centres - North American &amp; European Datacentres</t>
+  </si>
+  <si>
+    <t>- ISO 9001:2015, ISO 27001:2013 and ISO 20000-1:2011 certifications</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ISO/IEC 27001:2013, ISO/IEC 27017</t>
+  </si>
+  <si>
+    <t>- No ISO certifications</t>
+  </si>
+  <si>
+    <t>- Microsoft Azure infrastructure with ISO/IEC 27018, SOC 2 and more certifications</t>
+  </si>
+  <si>
+    <t>Pen tested by Fidus</t>
+  </si>
+  <si>
+    <t>Custom Roles</t>
+  </si>
+  <si>
+    <t>Ability to granularly control user access</t>
+  </si>
+  <si>
+    <t>As a product owner I want to be able to define user roles and permissions so that I can control levels of access to the CMS platform.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Custom roles only available in Enterprise plans</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Y
+In all plans
+</t>
+  </si>
+  <si>
+    <t>Custom roles for all plans</t>
+  </si>
+  <si>
+    <t>Pen Testing</t>
+  </si>
+  <si>
+    <t>Validate that that service has undertaken security assurances</t>
+  </si>
+  <si>
+    <t>As a product owner I want to know that the platform is regularly assessed for risks and vulnerabilities so that I know it is secure to deliver my service.</t>
+  </si>
+  <si>
+    <t>Y 
+(annual)</t>
+  </si>
+  <si>
+    <t>Y
+- Biannual Vulnerability Assessment and Penetration Testing (VAPT)</t>
+  </si>
+  <si>
+    <t>Annually</t>
+  </si>
+  <si>
+    <t>SSO</t>
+  </si>
+  <si>
+    <t>Ability to integrate with other identity services (e.g SAML 2.0 or Oauth)</t>
+  </si>
+  <si>
+    <t>As a product owner I want to be able to integrate my organisational SSO with the CMS platform so that users can use their corporate identity to access the platorm.</t>
+  </si>
+  <si>
+    <t>Only for enterprise plan</t>
+  </si>
+  <si>
+    <t>SSO with SAML 2.0</t>
+  </si>
+  <si>
+    <t>Single Sign-On for Enterprise plans</t>
+  </si>
+  <si>
+    <t>- Single-Sign-On for all plans</t>
+  </si>
+  <si>
+    <t>Third party sign on</t>
+  </si>
+  <si>
+    <t>Encryption (transit and rest)</t>
+  </si>
+  <si>
+    <t>Ensure all data is securley encrypted in transit and at rest (e.g TLS 1.2)</t>
+  </si>
+  <si>
+    <t>As a product owner I want to keep data secure when being transferred over a network so that we minimise data breaches and risk.</t>
+  </si>
+  <si>
+    <t>Y
+- 256-bit encryption of data in transit and at rest</t>
+  </si>
+  <si>
+    <t>- Data transferred between Prismic AWS EC2 instances and S3 storage facilities is secured via SSL endpoints using the HTTPS protocol. all Content Data is stored On disks in an encrypted manner (encrypted at rest)</t>
+  </si>
+  <si>
+    <t>- Data encryption at rest with 256-bit SSL encryption in transit</t>
+  </si>
+  <si>
+    <t>- Data transfer encryption (TLS 1.2)</t>
+  </si>
+  <si>
+    <t>Security Reporting</t>
+  </si>
+  <si>
+    <t>Insight report into security status and vulnerabilities of the service</t>
+  </si>
+  <si>
+    <t>As a product owner I want regular reports about the security health of the CMS platform so that I know it is secure and that vulnerabilities can be addressed.</t>
+  </si>
+  <si>
+    <t>Usage and activity reports</t>
+  </si>
+  <si>
+    <t>Uses Azure Monitoring</t>
+  </si>
+  <si>
+    <t>Data Soverignty</t>
+  </si>
+  <si>
+    <t>Location where the data is hosted and is subject to location data processsing policy and laws (e.g. GDPR)</t>
+  </si>
+  <si>
+    <t>As a product owner I want my service to be hosted in a secure compliant regional location so that I know my data and service will be secure by laws.</t>
+  </si>
+  <si>
+    <t>USA (Primary) &amp; EU (Backup)
+- Data is all hosted in North America, which could be an issue for any sensitive content</t>
+  </si>
+  <si>
+    <t>EU &amp; USA</t>
+  </si>
+  <si>
+    <t>Can choose - EU/USA/AUS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Data hosted in AWS facilities in Virginia, USA </t>
+  </si>
+  <si>
+    <t>Multi Region</t>
+  </si>
+  <si>
+    <t>On own infrastructure</t>
+  </si>
+  <si>
+    <t>Customer Support</t>
+  </si>
+  <si>
+    <t>First-line and technical support offered to the  organisation</t>
+  </si>
+  <si>
+    <t>As a product owner I want helpdesk support for the CMS platform so that if there any technical issues I can access support.</t>
+  </si>
+  <si>
+    <t>- Direct support only available for Enterprise plans.</t>
+  </si>
+  <si>
+    <t>Y
+- All Contentstack customers receive 24hr (Mon-Fri) support with average response times under 5 minutes. Enterprise plan includes 24/7 support.</t>
+  </si>
+  <si>
+    <t>Y
+- Priority chat and email for Business plan and 24/7x365 chat, email and phone for Enterprise
+- Service availability starts at 99.5% for Enterprise plans</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Y
+Priority Support in Platinum plan
+</t>
+  </si>
+  <si>
+    <t>-16h/day (Mon-Fri) in Professional plan</t>
+  </si>
+  <si>
+    <t>Y 
+(Community support)</t>
+  </si>
+  <si>
+    <t>Usability</t>
+  </si>
+  <si>
+    <t>Intuitive and easy to use with mininal training, configurable and accessible for users.</t>
+  </si>
+  <si>
+    <t>As a product owner I want the CMS platform to be easy to use so that I don't need specialist support.</t>
+  </si>
+  <si>
+    <t>- Simple to use WYSIWYG rich text editor
+- Simple content previewing</t>
+  </si>
+  <si>
+    <t>- WYSIWYG rich text editor
+- Content previewing requires publishing to a  "Preview" environment rather than there being a one click preview option (reducing the ease slightly)</t>
+  </si>
+  <si>
+    <t>- WYSIWYG rich text editor
+- Content previewing with in-browser editing</t>
+  </si>
+  <si>
+    <t>- WYSIWYG rich text editor
+- Drag and drop visual editing
+- Content previewing with in-browser editing feature
+- Page tagging and filtering</t>
+  </si>
+  <si>
+    <t>- WYSIWYG rich text editor
+- Content previewing</t>
+  </si>
+  <si>
+    <t>- WYSIWYG rich text editor
+- Content previewing including mobile devices
+- Drag and drop visual editing
+- Clean Copy &amp; Paste from Microsoft Word</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- WYSIWYG rich text editor
+</t>
+  </si>
+  <si>
+    <t>Uptime SLA's</t>
+  </si>
+  <si>
+    <t>Availablity and reliability of the service and how quick it is to recover and restore from and outage</t>
+  </si>
+  <si>
+    <t>As a product owner I want the CMS platform to have high availablity so that I can avoid a loss of service or downtime.</t>
+  </si>
+  <si>
+    <t>Y
+- SLA (99,9% API Uptime) 
+- 99.95% of API Uptime in Enterprise version</t>
+  </si>
+  <si>
+    <t>Y (99.9%)</t>
+  </si>
+  <si>
+    <t>PaaS dependent (by design)</t>
+  </si>
+  <si>
+    <t>Other Factors</t>
+  </si>
+  <si>
+    <t>Prices competitive at the mid and enterprise levels. Kontent is an option to give further consideration if looking to invest in the additional functionality that comes with a more premium plan.</t>
+  </si>
+  <si>
+    <t>Lack of ISO certifications rule this vendor out as an option at present. But the prices and features appear very competitive at this mid-level so Cosmic JS may be an option to reconsider in the future.</t>
+  </si>
+  <si>
+    <t>Not compatible with Ruby on Rails (.NET platform).
+Seems to be a decoupled rather than "API-first" headless CMS</t>
+  </si>
+  <si>
+    <t>Existing DfE Experience</t>
+  </si>
+  <si>
+    <t>As a product owner I want to reuse existing CMS patterns, templates and workflows so that I minimise the development time for my service.</t>
+  </si>
+  <si>
+    <t>-ILR
+-Apprenticeship Fire it up
+-Service Manual team</t>
+  </si>
+  <si>
+    <t>No known experience.</t>
+  </si>
+  <si>
+    <t>Used by National Careers Service team.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2141,6 +2873,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -2195,7 +2935,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2340,6 +3080,63 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2624,23 +3421,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" customWidth="1"/>
-    <col min="2" max="2" width="29.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.28515625" style="14" customWidth="1"/>
-    <col min="4" max="4" width="68.85546875" style="14" customWidth="1"/>
+    <col min="1" max="1" width="5.44140625" customWidth="1"/>
+    <col min="2" max="2" width="29.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.33203125" style="14" customWidth="1"/>
+    <col min="4" max="4" width="68.88671875" style="14" customWidth="1"/>
     <col min="5" max="5" width="12" style="12" customWidth="1"/>
-    <col min="6" max="6" width="23.28515625" customWidth="1"/>
-    <col min="7" max="7" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.7109375" customWidth="1"/>
+    <col min="6" max="6" width="23.33203125" customWidth="1"/>
+    <col min="7" max="7" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
       <c r="F2" s="3" t="s">
         <v>0</v>
       </c>
@@ -2651,7 +3448,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B3" s="16" t="s">
         <v>3</v>
       </c>
@@ -2668,7 +3465,7 @@
       <c r="G3" s="2"/>
       <c r="H3" s="32"/>
     </row>
-    <row r="4" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B4" s="17" t="s">
         <v>7</v>
       </c>
@@ -2691,7 +3488,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B5" s="17" t="s">
         <v>12</v>
       </c>
@@ -2714,7 +3511,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B6" s="17" t="s">
         <v>16</v>
       </c>
@@ -2737,7 +3534,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B7" s="17" t="s">
         <v>21</v>
       </c>
@@ -2760,7 +3557,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B8" s="17" t="s">
         <v>24</v>
       </c>
@@ -2783,7 +3580,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B9" s="17" t="s">
         <v>27</v>
       </c>
@@ -2806,7 +3603,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B10" s="17" t="s">
         <v>30</v>
       </c>
@@ -2829,7 +3626,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B11" s="19" t="s">
         <v>33</v>
       </c>
@@ -2840,7 +3637,7 @@
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
     </row>
-    <row r="12" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B12" s="17" t="s">
         <v>34</v>
       </c>
@@ -2863,7 +3660,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B13" s="17" t="s">
         <v>38</v>
       </c>
@@ -2886,7 +3683,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B14" s="17" t="s">
         <v>41</v>
       </c>
@@ -2909,7 +3706,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B15" s="17" t="s">
         <v>44</v>
       </c>
@@ -2932,7 +3729,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B16" s="17" t="s">
         <v>48</v>
       </c>
@@ -2955,7 +3752,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="17" t="s">
         <v>51</v>
       </c>
@@ -2978,7 +3775,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B18" s="17" t="s">
         <v>53</v>
       </c>
@@ -3001,7 +3798,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B19" s="17" t="s">
         <v>55</v>
       </c>
@@ -3024,7 +3821,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B20" s="19" t="s">
         <v>58</v>
       </c>
@@ -3035,7 +3832,7 @@
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
     </row>
-    <row r="21" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B21" s="17" t="s">
         <v>59</v>
       </c>
@@ -3058,7 +3855,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B22" s="17" t="s">
         <v>62</v>
       </c>
@@ -3081,7 +3878,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B23" s="17" t="s">
         <v>65</v>
       </c>
@@ -3104,7 +3901,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B24" s="17" t="s">
         <v>68</v>
       </c>
@@ -3127,7 +3924,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B25" s="17" t="s">
         <v>71</v>
       </c>
@@ -3150,7 +3947,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="2:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B26" s="17" t="s">
         <v>74</v>
       </c>
@@ -3173,7 +3970,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B27" s="17" t="s">
         <v>77</v>
       </c>
@@ -3196,7 +3993,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B28" s="17" t="s">
         <v>80</v>
       </c>
@@ -3219,7 +4016,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>83</v>
       </c>
@@ -3230,7 +4027,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>86</v>
       </c>
@@ -3249,6 +4046,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98D38F71-65DB-42D2-9179-80C1A6B69FBD}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:M32"/>
   <sheetViews>
@@ -3256,21 +4065,21 @@
       <selection activeCell="K43" sqref="K43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="3" width="35.85546875" customWidth="1"/>
-    <col min="4" max="5" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="35.88671875" customWidth="1"/>
+    <col min="4" max="5" width="28.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.7109375" customWidth="1"/>
+    <col min="7" max="7" width="24.6640625" customWidth="1"/>
     <col min="8" max="8" width="33" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="44.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.5703125" customWidth="1"/>
-    <col min="12" max="12" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="44.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.5546875" customWidth="1"/>
+    <col min="12" max="12" width="33.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="35.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.3">
       <c r="D2" s="5" t="s">
         <v>88</v>
       </c>
@@ -3302,7 +4111,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>97</v>
       </c>
@@ -3322,7 +4131,7 @@
       <c r="L3" s="7"/>
       <c r="M3" s="7"/>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>100</v>
       </c>
@@ -3358,7 +4167,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>102</v>
       </c>
@@ -3394,7 +4203,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
@@ -3410,7 +4219,7 @@
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
@@ -3426,7 +4235,7 @@
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
         <v>16</v>
       </c>
@@ -3446,7 +4255,7 @@
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
         <v>21</v>
       </c>
@@ -3466,7 +4275,7 @@
       <c r="L9" s="4"/>
       <c r="M9" s="4"/>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
         <v>24</v>
       </c>
@@ -3486,7 +4295,7 @@
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
         <v>27</v>
       </c>
@@ -3506,7 +4315,7 @@
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
         <v>30</v>
       </c>
@@ -3526,7 +4335,7 @@
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
         <v>33</v>
       </c>
@@ -3542,7 +4351,7 @@
       <c r="L13" s="5"/>
       <c r="M13" s="5"/>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
         <v>34</v>
       </c>
@@ -3562,7 +4371,7 @@
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
         <v>38</v>
       </c>
@@ -3582,7 +4391,7 @@
       <c r="L15" s="4"/>
       <c r="M15" s="4"/>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
         <v>41</v>
       </c>
@@ -3598,7 +4407,7 @@
       <c r="L16" s="4"/>
       <c r="M16" s="4"/>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
         <v>44</v>
       </c>
@@ -3614,7 +4423,7 @@
       <c r="L17" s="4"/>
       <c r="M17" s="4"/>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
         <v>48</v>
       </c>
@@ -3630,7 +4439,7 @@
       <c r="L18" s="4"/>
       <c r="M18" s="4"/>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
         <v>51</v>
       </c>
@@ -3646,7 +4455,7 @@
       <c r="L19" s="4"/>
       <c r="M19" s="4"/>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
         <v>53</v>
       </c>
@@ -3662,7 +4471,7 @@
       <c r="L20" s="4"/>
       <c r="M20" s="4"/>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
         <v>55</v>
       </c>
@@ -3682,7 +4491,7 @@
       <c r="L21" s="4"/>
       <c r="M21" s="4"/>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B22" s="2" t="s">
         <v>58</v>
       </c>
@@ -3698,7 +4507,7 @@
       <c r="L22" s="5"/>
       <c r="M22" s="5"/>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B23" s="1" t="s">
         <v>59</v>
       </c>
@@ -3714,7 +4523,7 @@
       <c r="L23" s="4"/>
       <c r="M23" s="4"/>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B24" s="1" t="s">
         <v>62</v>
       </c>
@@ -3734,7 +4543,7 @@
       <c r="L24" s="4"/>
       <c r="M24" s="4"/>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B25" s="1" t="s">
         <v>65</v>
       </c>
@@ -3754,7 +4563,7 @@
       <c r="L25" s="4"/>
       <c r="M25" s="4"/>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B26" s="1" t="s">
         <v>68</v>
       </c>
@@ -3770,7 +4579,7 @@
       <c r="L26" s="4"/>
       <c r="M26" s="4"/>
     </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B27" s="1" t="s">
         <v>71</v>
       </c>
@@ -3786,7 +4595,7 @@
       <c r="L27" s="4"/>
       <c r="M27" s="4"/>
     </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B28" s="1" t="s">
         <v>74</v>
       </c>
@@ -3802,7 +4611,7 @@
       <c r="L28" s="4"/>
       <c r="M28" s="4"/>
     </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B29" s="1" t="s">
         <v>77</v>
       </c>
@@ -3818,7 +4627,7 @@
       <c r="L29" s="4"/>
       <c r="M29" s="4"/>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B30" s="1" t="s">
         <v>80</v>
       </c>
@@ -3834,7 +4643,7 @@
       <c r="L30" s="4"/>
       <c r="M30" s="4"/>
     </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B31" s="2" t="s">
         <v>106</v>
       </c>
@@ -3850,7 +4659,7 @@
       <c r="L31" s="9"/>
       <c r="M31" s="9"/>
     </row>
-    <row r="32" spans="2:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:13" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="11" t="s">
         <v>107</v>
       </c>
@@ -3883,7 +4692,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:K17"/>
   <sheetViews>
@@ -3891,20 +4700,20 @@
       <selection activeCell="F4" sqref="F4:F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.42578125" style="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" style="27" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.28515625" customWidth="1"/>
-    <col min="8" max="9" width="24.7109375" customWidth="1"/>
-    <col min="10" max="10" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.7109375" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.6640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.44140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" style="27" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.33203125" customWidth="1"/>
+    <col min="8" max="9" width="24.6640625" customWidth="1"/>
+    <col min="10" max="10" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
       <c r="F2" s="3" t="s">
         <v>113</v>
       </c>
@@ -3924,7 +4733,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>118</v>
       </c>
@@ -3946,7 +4755,7 @@
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="2:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B4" s="11" t="s">
         <v>120</v>
       </c>
@@ -3978,7 +4787,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="2:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B5" s="11" t="s">
         <v>123</v>
       </c>
@@ -4010,7 +4819,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="2:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B6" s="11" t="s">
         <v>126</v>
       </c>
@@ -4042,7 +4851,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="2:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B7" s="11" t="s">
         <v>129</v>
       </c>
@@ -4074,7 +4883,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="2:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B8" s="11" t="s">
         <v>132</v>
       </c>
@@ -4106,7 +4915,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="2:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B9" s="11" t="s">
         <v>135</v>
       </c>
@@ -4138,7 +4947,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="2:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B10" s="11" t="s">
         <v>138</v>
       </c>
@@ -4170,7 +4979,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="2:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B11" s="11" t="s">
         <v>141</v>
       </c>
@@ -4202,7 +5011,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="2:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B12" s="11" t="s">
         <v>144</v>
       </c>
@@ -4234,7 +5043,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="2:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B13" s="11" t="s">
         <v>147</v>
       </c>
@@ -4266,7 +5075,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="2:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B14" s="11" t="s">
         <v>150</v>
       </c>
@@ -4298,7 +5107,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="2:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B15" s="28" t="s">
         <v>153</v>
       </c>
@@ -4330,7 +5139,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D17" s="43"/>
     </row>
   </sheetData>
@@ -4339,7 +5148,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B2:J20"/>
   <sheetViews>
@@ -4347,20 +5156,20 @@
       <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="60.7109375" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" customWidth="1"/>
-    <col min="4" max="4" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.28515625" customWidth="1"/>
-    <col min="10" max="10" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="60.6640625" customWidth="1"/>
+    <col min="3" max="3" width="18.5546875" customWidth="1"/>
+    <col min="4" max="4" width="31.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.33203125" customWidth="1"/>
+    <col min="10" max="10" width="29.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C2" s="25" t="s">
         <v>157</v>
       </c>
@@ -4386,7 +5195,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
       <c r="E3" s="30"/>
@@ -4396,7 +5205,7 @@
       <c r="I3" s="30"/>
       <c r="J3" s="30"/>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C4" s="25"/>
       <c r="D4" s="25"/>
       <c r="E4" s="25"/>
@@ -4406,7 +5215,7 @@
       <c r="I4" s="25"/>
       <c r="J4" s="25"/>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C5" s="25" t="s">
         <v>104</v>
       </c>
@@ -4432,7 +5241,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>118</v>
       </c>
@@ -4445,7 +5254,7 @@
       <c r="I6" s="23"/>
       <c r="J6" s="23"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B7" s="11" t="s">
         <v>120</v>
       </c>
@@ -4458,7 +5267,7 @@
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B8" s="11" t="s">
         <v>123</v>
       </c>
@@ -4471,7 +5280,7 @@
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B9" s="11" t="s">
         <v>126</v>
       </c>
@@ -4484,7 +5293,7 @@
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B10" s="11" t="s">
         <v>129</v>
       </c>
@@ -4497,7 +5306,7 @@
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B11" s="11" t="s">
         <v>132</v>
       </c>
@@ -4510,7 +5319,7 @@
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B12" s="11" t="s">
         <v>135</v>
       </c>
@@ -4523,7 +5332,7 @@
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B13" s="11" t="s">
         <v>138</v>
       </c>
@@ -4536,7 +5345,7 @@
       <c r="I13" s="29"/>
       <c r="J13" s="29"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B14" s="11" t="s">
         <v>141</v>
       </c>
@@ -4549,7 +5358,7 @@
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B15" s="11" t="s">
         <v>144</v>
       </c>
@@ -4562,7 +5371,7 @@
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B16" s="11" t="s">
         <v>147</v>
       </c>
@@ -4575,7 +5384,7 @@
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B17" s="11" t="s">
         <v>150</v>
       </c>
@@ -4588,7 +5397,7 @@
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B18" s="28" t="s">
         <v>153</v>
       </c>
@@ -4601,7 +5410,7 @@
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
         <v>106</v>
       </c>
@@ -4614,7 +5423,7 @@
       <c r="I19" s="9"/>
       <c r="J19" s="9"/>
     </row>
-    <row r="20" spans="2:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B20" s="11" t="s">
         <v>107</v>
       </c>
@@ -4637,7 +5446,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B2:M19"/>
   <sheetViews>
@@ -4645,22 +5454,22 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31" style="42" customWidth="1"/>
     <col min="4" max="4" width="47" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" customWidth="1"/>
-    <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.85546875" customWidth="1"/>
+    <col min="7" max="7" width="15.88671875" customWidth="1"/>
+    <col min="8" max="8" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.88671875" customWidth="1"/>
     <col min="10" max="10" width="19" customWidth="1"/>
-    <col min="11" max="11" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.28515625" customWidth="1"/>
+    <col min="11" max="11" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B2" s="33"/>
       <c r="C2" s="40"/>
       <c r="D2" s="35"/>
@@ -4688,7 +5497,7 @@
       </c>
       <c r="M2" s="33"/>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B3" s="33"/>
       <c r="C3" s="40"/>
       <c r="D3" s="35"/>
@@ -4716,7 +5525,7 @@
       </c>
       <c r="M3" s="33"/>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B4" s="33"/>
       <c r="C4" s="40"/>
       <c r="D4" s="35"/>
@@ -4730,7 +5539,7 @@
       <c r="L4" s="34"/>
       <c r="M4" s="33"/>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B5" s="34" t="s">
         <v>177</v>
       </c>
@@ -4752,7 +5561,7 @@
       <c r="L5" s="34"/>
       <c r="M5" s="33"/>
     </row>
-    <row r="6" spans="2:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B6" s="17" t="s">
         <v>178</v>
       </c>
@@ -4788,7 +5597,7 @@
       </c>
       <c r="M6" s="33"/>
     </row>
-    <row r="7" spans="2:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B7" s="17" t="s">
         <v>182</v>
       </c>
@@ -4824,7 +5633,7 @@
       </c>
       <c r="M7" s="33"/>
     </row>
-    <row r="8" spans="2:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B8" s="17" t="s">
         <v>185</v>
       </c>
@@ -4860,7 +5669,7 @@
       </c>
       <c r="M8" s="33"/>
     </row>
-    <row r="9" spans="2:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B9" s="17" t="s">
         <v>169</v>
       </c>
@@ -4896,7 +5705,7 @@
       </c>
       <c r="M9" s="33"/>
     </row>
-    <row r="10" spans="2:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B10" s="17" t="s">
         <v>190</v>
       </c>
@@ -4932,7 +5741,7 @@
       </c>
       <c r="M10" s="33"/>
     </row>
-    <row r="11" spans="2:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B11" s="17" t="s">
         <v>193</v>
       </c>
@@ -4968,7 +5777,7 @@
       </c>
       <c r="M11" s="33"/>
     </row>
-    <row r="12" spans="2:13" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:13" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="17" t="s">
         <v>196</v>
       </c>
@@ -5004,7 +5813,7 @@
       </c>
       <c r="M12" s="33"/>
     </row>
-    <row r="13" spans="2:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B13" s="17" t="s">
         <v>200</v>
       </c>
@@ -5040,7 +5849,7 @@
       </c>
       <c r="M13" s="33"/>
     </row>
-    <row r="14" spans="2:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B14" s="17" t="s">
         <v>203</v>
       </c>
@@ -5076,7 +5885,7 @@
       </c>
       <c r="M14" s="33"/>
     </row>
-    <row r="15" spans="2:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B15" s="17" t="s">
         <v>207</v>
       </c>
@@ -5112,7 +5921,7 @@
       </c>
       <c r="M15" s="33"/>
     </row>
-    <row r="16" spans="2:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B16" s="17" t="s">
         <v>211</v>
       </c>
@@ -5148,7 +5957,7 @@
       </c>
       <c r="M16" s="33"/>
     </row>
-    <row r="17" spans="2:13" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:13" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="17" t="s">
         <v>214</v>
       </c>
@@ -5184,7 +5993,7 @@
       </c>
       <c r="M17" s="33"/>
     </row>
-    <row r="18" spans="2:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B18" s="17" t="s">
         <v>217</v>
       </c>
@@ -5220,7 +6029,7 @@
       </c>
       <c r="M18" s="33"/>
     </row>
-    <row r="19" spans="2:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B19" s="37" t="s">
         <v>220</v>
       </c>
@@ -5262,7 +6071,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="B2:P23"/>
   <sheetViews>
@@ -5270,19 +6079,19 @@
       <selection activeCell="P1" sqref="P1:P1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" customWidth="1"/>
-    <col min="5" max="5" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15.88671875" customWidth="1"/>
+    <col min="5" max="5" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.88671875" customWidth="1"/>
     <col min="7" max="7" width="19" customWidth="1"/>
-    <col min="8" max="8" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="15" width="20.28515625" customWidth="1"/>
+    <col min="8" max="8" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="15" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" s="44" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:16" s="44" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C2" s="36" t="s">
         <v>223</v>
       </c>
@@ -5323,7 +6132,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B3" s="33"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -5340,7 +6149,7 @@
       <c r="O3" s="5"/>
       <c r="P3" s="33"/>
     </row>
-    <row r="4" spans="2:16" s="46" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:16" s="46" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C4" s="25" t="s">
         <v>168</v>
       </c>
@@ -5381,7 +6190,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B5" s="34" t="s">
         <v>118</v>
       </c>
@@ -5400,7 +6209,7 @@
       <c r="O5" s="34"/>
       <c r="P5" s="33"/>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B6" s="17" t="s">
         <v>178</v>
       </c>
@@ -5423,7 +6232,7 @@
       <c r="O6" s="4"/>
       <c r="P6" s="33"/>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B7" s="17" t="s">
         <v>182</v>
       </c>
@@ -5446,7 +6255,7 @@
       <c r="O7" s="4"/>
       <c r="P7" s="33"/>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B8" s="17" t="s">
         <v>185</v>
       </c>
@@ -5469,7 +6278,7 @@
       <c r="O8" s="4"/>
       <c r="P8" s="33"/>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B9" s="17" t="s">
         <v>169</v>
       </c>
@@ -5492,7 +6301,7 @@
       <c r="O9" s="4"/>
       <c r="P9" s="33"/>
     </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B10" s="17" t="s">
         <v>190</v>
       </c>
@@ -5515,7 +6324,7 @@
       <c r="O10" s="4"/>
       <c r="P10" s="33"/>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B11" s="17" t="s">
         <v>193</v>
       </c>
@@ -5538,7 +6347,7 @@
       <c r="O11" s="4"/>
       <c r="P11" s="33"/>
     </row>
-    <row r="12" spans="2:16" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:16" ht="41.4" x14ac:dyDescent="0.3">
       <c r="B12" s="17" t="s">
         <v>196</v>
       </c>
@@ -5561,7 +6370,7 @@
       <c r="O12" s="10"/>
       <c r="P12" s="33"/>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B13" s="17" t="s">
         <v>200</v>
       </c>
@@ -5584,7 +6393,7 @@
       <c r="O13" s="4"/>
       <c r="P13" s="33"/>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B14" s="17" t="s">
         <v>203</v>
       </c>
@@ -5607,7 +6416,7 @@
       <c r="O14" s="10"/>
       <c r="P14" s="33"/>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B15" s="17" t="s">
         <v>207</v>
       </c>
@@ -5630,7 +6439,7 @@
       <c r="O15" s="4"/>
       <c r="P15" s="33"/>
     </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B16" s="17" t="s">
         <v>211</v>
       </c>
@@ -5653,7 +6462,7 @@
       <c r="O16" s="4"/>
       <c r="P16" s="33"/>
     </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B17" s="17" t="s">
         <v>214</v>
       </c>
@@ -5676,7 +6485,7 @@
       <c r="O17" s="4"/>
       <c r="P17" s="33"/>
     </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B18" s="17" t="s">
         <v>217</v>
       </c>
@@ -5699,7 +6508,7 @@
       <c r="O18" s="4"/>
       <c r="P18" s="33"/>
     </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B19" s="37" t="s">
         <v>220</v>
       </c>
@@ -5722,22 +6531,22 @@
       <c r="O19" s="4"/>
       <c r="P19" s="33"/>
     </row>
-    <row r="20" spans="2:16" ht="135" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:16" ht="115.2" x14ac:dyDescent="0.3">
       <c r="K20" s="48" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="21" spans="2:16" ht="90" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:16" ht="86.4" x14ac:dyDescent="0.3">
       <c r="K21" s="49" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="22" spans="2:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:16" ht="43.2" x14ac:dyDescent="0.3">
       <c r="K22" s="50" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="23" spans="2:16" ht="75" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:16" ht="72" x14ac:dyDescent="0.3">
       <c r="K23" s="50" t="s">
         <v>244</v>
       </c>
@@ -5753,22 +6562,1085 @@
 </worksheet>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77CFD866-DE87-41D5-BE31-43FB6D2DE716}">
+  <dimension ref="B2:L32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="28.77734375" style="68" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.88671875" style="14" customWidth="1"/>
+    <col min="4" max="4" width="38.21875" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" customWidth="1"/>
+    <col min="6" max="6" width="31.44140625" customWidth="1"/>
+    <col min="7" max="7" width="28.6640625" customWidth="1"/>
+    <col min="8" max="8" width="36.5546875" customWidth="1"/>
+    <col min="9" max="10" width="30.21875" customWidth="1"/>
+    <col min="11" max="11" width="34.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="31.21875" style="69" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:12" s="14" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B2" s="15" t="s">
+        <v>245</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="36" t="s">
+        <v>246</v>
+      </c>
+      <c r="G2" s="36" t="s">
+        <v>247</v>
+      </c>
+      <c r="H2" s="36" t="s">
+        <v>248</v>
+      </c>
+      <c r="I2" s="36" t="s">
+        <v>249</v>
+      </c>
+      <c r="J2" s="36" t="s">
+        <v>250</v>
+      </c>
+      <c r="K2" s="36" t="s">
+        <v>251</v>
+      </c>
+      <c r="L2" s="36" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B3" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="52" t="s">
+        <v>254</v>
+      </c>
+      <c r="G3" s="53" t="s">
+        <v>255</v>
+      </c>
+      <c r="H3" s="52" t="s">
+        <v>256</v>
+      </c>
+      <c r="I3" s="52" t="s">
+        <v>257</v>
+      </c>
+      <c r="J3" s="52" t="s">
+        <v>258</v>
+      </c>
+      <c r="K3" s="52" t="s">
+        <v>259</v>
+      </c>
+      <c r="L3" s="54" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" ht="409.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="55" t="s">
+        <v>261</v>
+      </c>
+      <c r="C4" s="51"/>
+      <c r="D4" s="56" t="s">
+        <v>262</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>263</v>
+      </c>
+      <c r="G4" s="18" t="s">
+        <v>264</v>
+      </c>
+      <c r="H4" s="40" t="s">
+        <v>265</v>
+      </c>
+      <c r="I4" s="57" t="s">
+        <v>266</v>
+      </c>
+      <c r="J4" s="57" t="s">
+        <v>267</v>
+      </c>
+      <c r="K4" s="18" t="s">
+        <v>268</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B5" s="55" t="s">
+        <v>270</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>271</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>273</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>273</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>273</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>273</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>273</v>
+      </c>
+      <c r="K5" s="10" t="s">
+        <v>273</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="55" t="s">
+        <v>275</v>
+      </c>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K6" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="L6" s="4"/>
+    </row>
+    <row r="7" spans="2:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B7" s="55" t="s">
+        <v>278</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>279</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B8" s="55" t="s">
+        <v>281</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>282</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>283</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L8" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="B9" s="55" t="s">
+        <v>284</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>285</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>286</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>287</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L9" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" ht="145.94999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="17" t="s">
+        <v>288</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>289</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="J10" s="10" t="s">
+        <v>294</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L10" s="10" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B11" s="55" t="s">
+        <v>296</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>297</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>298</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>299</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L11" s="58" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B12" s="55" t="s">
+        <v>300</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>301</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>302</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L12" s="58" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B13" s="55" t="s">
+        <v>303</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>304</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>305</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L13" s="59" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B14" s="55" t="s">
+        <v>306</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>307</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>308</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L14" s="58" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B15" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>310</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>311</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L15" s="59" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B16" s="17" t="s">
+        <v>312</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>313</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>314</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="I16" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="J16" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="K16" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="L16" s="59" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" ht="270.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="17" t="s">
+        <v>315</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>316</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>314</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="60" t="s">
+        <v>317</v>
+      </c>
+      <c r="G17" s="61" t="s">
+        <v>318</v>
+      </c>
+      <c r="H17" s="61" t="s">
+        <v>319</v>
+      </c>
+      <c r="I17" s="61" t="s">
+        <v>320</v>
+      </c>
+      <c r="J17" s="61" t="s">
+        <v>321</v>
+      </c>
+      <c r="K17" s="61" t="s">
+        <v>322</v>
+      </c>
+      <c r="L17" s="62" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" ht="166.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="18" t="s">
+        <v>324</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>325</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>326</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F18" s="61" t="s">
+        <v>327</v>
+      </c>
+      <c r="G18" s="61" t="s">
+        <v>328</v>
+      </c>
+      <c r="H18" s="61" t="s">
+        <v>329</v>
+      </c>
+      <c r="I18" s="61" t="s">
+        <v>330</v>
+      </c>
+      <c r="J18" s="61" t="s">
+        <v>329</v>
+      </c>
+      <c r="K18" s="61" t="s">
+        <v>331</v>
+      </c>
+      <c r="L18" s="62" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" ht="72" x14ac:dyDescent="0.3">
+      <c r="B19" s="13" t="s">
+        <v>333</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>334</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>335</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J19" s="63" t="s">
+        <v>336</v>
+      </c>
+      <c r="K19" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L19" s="59" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B20" s="11" t="s">
+        <v>337</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>338</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>339</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>340</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H20" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="I20" s="10" t="s">
+        <v>342</v>
+      </c>
+      <c r="J20" s="64" t="s">
+        <v>343</v>
+      </c>
+      <c r="K20" s="64" t="s">
+        <v>344</v>
+      </c>
+      <c r="L20" s="59" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" ht="72" x14ac:dyDescent="0.3">
+      <c r="B21" s="11" t="s">
+        <v>346</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>347</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>348</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" s="65" t="s">
+        <v>349</v>
+      </c>
+      <c r="G21" s="65" t="s">
+        <v>350</v>
+      </c>
+      <c r="H21" s="65" t="s">
+        <v>351</v>
+      </c>
+      <c r="I21" s="65" t="s">
+        <v>352</v>
+      </c>
+      <c r="J21" s="66" t="s">
+        <v>353</v>
+      </c>
+      <c r="K21" s="67" t="s">
+        <v>354</v>
+      </c>
+      <c r="L21" s="62" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B22" s="17" t="s">
+        <v>356</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>357</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>358</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>359</v>
+      </c>
+      <c r="G22" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K22" s="4" t="s">
+        <v>361</v>
+      </c>
+      <c r="L22" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B23" s="11" t="s">
+        <v>362</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>363</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>364</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>365</v>
+      </c>
+      <c r="G23" s="64" t="s">
+        <v>366</v>
+      </c>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4" t="s">
+        <v>367</v>
+      </c>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B24" s="11" t="s">
+        <v>368</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>369</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>370</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>373</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>373</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="K24" s="63" t="s">
+        <v>374</v>
+      </c>
+      <c r="L24" s="59" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="B25" s="13" t="s">
+        <v>376</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>377</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>378</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G25" s="10" t="s">
+        <v>379</v>
+      </c>
+      <c r="H25" s="4"/>
+      <c r="I25" s="64" t="s">
+        <v>380</v>
+      </c>
+      <c r="J25" s="64" t="s">
+        <v>381</v>
+      </c>
+      <c r="K25" s="63" t="s">
+        <v>382</v>
+      </c>
+      <c r="L25" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B26" s="11" t="s">
+        <v>383</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>384</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>385</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="K26" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L26" s="59" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B27" s="11" t="s">
+        <v>388</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>389</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>390</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>391</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="I27" s="64" t="s">
+        <v>394</v>
+      </c>
+      <c r="J27" s="4" t="s">
+        <v>395</v>
+      </c>
+      <c r="K27" s="4" t="s">
+        <v>395</v>
+      </c>
+      <c r="L27" s="4" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="B28" s="11" t="s">
+        <v>397</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>399</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F28" s="61" t="s">
+        <v>400</v>
+      </c>
+      <c r="G28" s="10" t="s">
+        <v>401</v>
+      </c>
+      <c r="H28" s="10" t="s">
+        <v>402</v>
+      </c>
+      <c r="I28" s="10" t="s">
+        <v>403</v>
+      </c>
+      <c r="J28" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K28" s="63" t="s">
+        <v>404</v>
+      </c>
+      <c r="L28" s="10" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" ht="119.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="17" t="s">
+        <v>406</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>407</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>408</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F29" s="61" t="s">
+        <v>409</v>
+      </c>
+      <c r="G29" s="61" t="s">
+        <v>410</v>
+      </c>
+      <c r="H29" s="61" t="s">
+        <v>411</v>
+      </c>
+      <c r="I29" s="61" t="s">
+        <v>412</v>
+      </c>
+      <c r="J29" s="61" t="s">
+        <v>413</v>
+      </c>
+      <c r="K29" s="61" t="s">
+        <v>414</v>
+      </c>
+      <c r="L29" s="61" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B30" s="11" t="s">
+        <v>416</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>417</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>418</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I30" s="10" t="s">
+        <v>419</v>
+      </c>
+      <c r="J30" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K30" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="L30" s="10" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" ht="112.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="11" t="s">
+        <v>422</v>
+      </c>
+      <c r="C31" s="51"/>
+      <c r="D31" s="51"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="18" t="s">
+        <v>423</v>
+      </c>
+      <c r="I31" s="4"/>
+      <c r="J31" s="18" t="s">
+        <v>424</v>
+      </c>
+      <c r="K31" s="61" t="s">
+        <v>425</v>
+      </c>
+      <c r="L31" s="58"/>
+    </row>
+    <row r="32" spans="2:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B32" s="11" t="s">
+        <v>426</v>
+      </c>
+      <c r="C32" s="51"/>
+      <c r="D32" s="13" t="s">
+        <v>427</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F32" s="64" t="s">
+        <v>428</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>429</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>429</v>
+      </c>
+      <c r="I32" s="4" t="s">
+        <v>429</v>
+      </c>
+      <c r="J32" s="4" t="s">
+        <v>429</v>
+      </c>
+      <c r="K32" s="4" t="s">
+        <v>430</v>
+      </c>
+      <c r="L32" s="10" t="s">
+        <v>430</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F3" r:id="rId1" xr:uid="{71BC4B22-CCEF-4EA5-8A95-5A3A4D4B5EF9}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{4F8CB76F-DCE3-43A8-97FB-7E485E0FC38D}"/>
+    <hyperlink ref="K3" r:id="rId3" xr:uid="{23C6D77B-538B-40AB-A6D4-772DDEB582BE}"/>
+    <hyperlink ref="I3" r:id="rId4" xr:uid="{55ED426A-5DA9-4E47-A769-89669434E55B}"/>
+    <hyperlink ref="H3" r:id="rId5" xr:uid="{FCB86B0D-9681-4F78-AD71-C398F6C5B7D4}"/>
+    <hyperlink ref="J3" r:id="rId6" xr:uid="{46F94EBA-7865-48C6-B065-4D110AE97818}"/>
+    <hyperlink ref="L3" r:id="rId7" xr:uid="{B6ABF243-587B-4246-8761-BB7C0832C12D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
+</worksheet>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B57151A7873D3B4CB38449F1E4CD2EAA" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7e8202c7bfeeae60ce525a5ca4d0fe6a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="161ae125-8199-47a3-b5d9-eda3a8f2a061" xmlns:ns4="680bcac6-b14c-4c2b-a58b-c019311aeaad" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1abf75ed68cd583d13418a16f207a9e6" ns3:_="" ns4:_="">
     <xsd:import namespace="161ae125-8199-47a3-b5d9-eda3a8f2a061"/>
@@ -5971,10 +7843,36 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FBD369E-6A68-4C96-8DEA-0EC45C5264AD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4651E139-BFC7-495A-9CCD-06709AD31B99}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="161ae125-8199-47a3-b5d9-eda3a8f2a061"/>
+    <ds:schemaRef ds:uri="680bcac6-b14c-4c2b-a58b-c019311aeaad"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5997,20 +7895,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4651E139-BFC7-495A-9CCD-06709AD31B99}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FBD369E-6A68-4C96-8DEA-0EC45C5264AD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="161ae125-8199-47a3-b5d9-eda3a8f2a061"/>
-    <ds:schemaRef ds:uri="680bcac6-b14c-4c2b-a58b-c019311aeaad"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Revert "Adding Content Management System content"
This reverts commit 1f190987e66d82a0a8fcec4f89152d199f0e1194.
</commit_message>
<xml_diff>
--- a/documents/common-component-matrix.xlsx
+++ b/documents/common-component-matrix.xlsx
@@ -1,26 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\github\architecture\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\DFE\Top15\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B1EE814-4381-496C-8184-565EDF3AA24F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AA99E81D-BD3E-4D7C-9BEE-B53C5EF7943F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="-120" windowWidth="25440" windowHeight="15390" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9060" yWindow="1740" windowWidth="25170" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping Applications" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="9" r:id="rId2"/>
-    <sheet name="Mapping Services" sheetId="4" r:id="rId3"/>
-    <sheet name="Postcode Applications" sheetId="5" r:id="rId4"/>
-    <sheet name="Postcode Services" sheetId="6" r:id="rId5"/>
-    <sheet name="Notification Application" sheetId="7" r:id="rId6"/>
-    <sheet name="Notification Services" sheetId="8" r:id="rId7"/>
-    <sheet name="CMS Applications" sheetId="11" r:id="rId8"/>
+    <sheet name="Mapping Services" sheetId="4" r:id="rId2"/>
+    <sheet name="Postcode Applications" sheetId="5" r:id="rId3"/>
+    <sheet name="Postcode Services" sheetId="6" r:id="rId4"/>
+    <sheet name="Notification Application" sheetId="7" r:id="rId5"/>
+    <sheet name="Notification Services" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -1265,7 +1263,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="991" uniqueCount="431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="245">
   <si>
     <t>Azure Maps</t>
   </si>
@@ -2053,742 +2051,12 @@
   <si>
     <t>https://dfedigital.atlassian.net/wiki/spaces/TSTL/pages/1223458929/What+we+use+and+defaults</t>
   </si>
-  <si>
-    <t>Feature</t>
-  </si>
-  <si>
-    <t>Contentful</t>
-  </si>
-  <si>
-    <t>Contentstack</t>
-  </si>
-  <si>
-    <t>Kontent</t>
-  </si>
-  <si>
-    <t>Prismic</t>
-  </si>
-  <si>
-    <t>Cosmic JS</t>
-  </si>
-  <si>
-    <t>Sitefinity</t>
-  </si>
-  <si>
-    <t>OrchardCore</t>
-  </si>
-  <si>
-    <t>Weblink</t>
-  </si>
-  <si>
-    <t>https://www.contentful.com/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.contentstack.com/ </t>
-  </si>
-  <si>
-    <t>https://kontent.ai/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://prismic.io/ </t>
-  </si>
-  <si>
-    <t>https://www.cosmicjs.com/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.progress.com/sitefinity-cms </t>
-  </si>
-  <si>
-    <t>http://www.orchardcore.net/</t>
-  </si>
-  <si>
-    <t>Licence Type/Pricing Structure</t>
-  </si>
-  <si>
-    <t>Dependent on usecases, specific requirements (inc. specialist language content) and size of service</t>
-  </si>
-  <si>
-    <t>•	On-demand = Pay for the space only
-•	Micro = €420/year (1 master and 1 sandbox environment, 1 role, 2 locales, 24 content types, 5,000 records)
-•	Small = €2,028/year (1 master and 2 sandbox environment, 2 role, 4 locales, 24 content types, 10,000 records)
-•	Medium = €5,268/year (1 master and 3 sandbox environment, 2 role, 7 locales, 48 content types, 25,000 records)
-•	Large = €9,468/year (1 master and 5 sandbox environment, 4 role, 10 locales, 48 content types, 50,000 records, plus GraphQL API)
-•	Enterprise = Pay for the platform + SLA + space
-•	Professional = €24,000+/year (+ space and SLA costs) - custom roles, SSO, full webhook functionality, scheduled publishing
-•	Scale = €90,000+/year (+ space and SLA costs)
-•	High availability = €225,000+/year (+ space and SLA costs)</t>
-  </si>
-  <si>
-    <t>•Business = $3,500/month
--10 Users
-- 1 Property
-- Content Types
-- Digital Assets Management
-- Rich Text Editor
-- Multiple Environments
-- Modular Blocks (Page Builder)
-- Custom Fields
-•Enterprise = Starts at $10,000/month (requires quotation) and onboarding fee required for first year
-- 10+ Users
-- 3+ Properties
-- Workflows
-- Grouped Releases
-- Bulk Operations
-- Experience Extensions (Integrations)
-- Dashboard
-- Analytics</t>
-  </si>
-  <si>
-    <t>•Starter = Free
-- 3 Users ($10/month per extra user. Max 20 users)
-- Unlimited projects (but without ability to clone)
-- 5,000 Content items
-- 2 Languages
-•Business = $999/month
-- 15 Users ($10/month per extra user. Max 30 users)
-- Unlimited projects
-- 25,000 Content items
-- 10 Languages
-- 1 predefined role + 2 Custom roles
-•Enterprise = Starts at $1,499/month (requires quotation)
-- Custom number of Users
-- Unlimited projects
-- More Content items
-- More Languages
-- More Custom roles</t>
-  </si>
-  <si>
-    <t>•Free and Starter are the cheapest tiers
-•Small = $20/month OR $15/month for annual contract
-- 7 Users
-- Basic Support
-- Core features
-•Professional - Medium = $125/month OR $100/month for annual contract
-- 25 Users
-- SLA (99,5% API Uptime), Basic Support
-- User roles, publication workflow &amp; collaboration features
-•Professional - Platinum = $575/month OR $500/month for annual contract
-- Unlimited users
-- SLA (99,5% API Uptime), Priority Support
-- User roles, publication workflow &amp; collaboration features
-•Enterprise = Starts at $24,000/year (requires quotation)
-- Includes three environments (development, staging, production)
-- SLA (99.95% API Uptime)
-- Daily backups &amp; snapshots
-- SSO and MFA</t>
-  </si>
-  <si>
-    <t>•	Personal Plan provides a free option
-•	Starter = $99/month (10% off for annual)
-- Single Bucket
-- 5 team members
-- 25,000 API requests
-- 10,000 files / 3GB media storage
-•	Pro = $299/month (10% off for annual)
-- Single Bucket
-- 10 team members
-- 150,000 API requests
-- 50,000 files / 15GB media storage
-•	Business = $799/month (10% off for annual)
-- Single Bucket
-- 30 team members
-- 500,000 API requests
-- 100,000 files / 50GB media storage
-•	Enterprise = requires quotation
-- Dedicated Infrastructure
-- Single Sign-on
-- 24/7 Support
-- SLA
-- Migration Support
-- All add-ons included
-- Company workspace</t>
-  </si>
-  <si>
-    <t>•	Professional Edition = Starts at $15,000/year (requires quotation)
-- 1 production domain or server
-- 10 concurrent users
-- Web Content Management
-- Developer Productivity Tools
-•	Online Marketing Edition = Starts at $30,000+/year (requires quotation)
-- 1 production domain
-- 15 concurrent users
-- Web Content Management
-- Developer Productivity Tools
-- Marketing and CRM connectors
-- Content personalisation
-•	Enterprise Edition = Starts at $50,000/year (requires quotation)
-- Unlimited concurrent users
-- Web Content Management
-- Developer Productivity Tools
-- All connectors
-- Content personalisation
-- Site sync between environments
-- Translations management
-- System audit trail</t>
-  </si>
-  <si>
-    <t>Opensource</t>
-  </si>
-  <si>
-    <t>Service Type</t>
-  </si>
-  <si>
-    <t>Cloud based or on Prem</t>
-  </si>
-  <si>
-    <t>As a product owner I want a CMS service to develop content so that I can publish digital content online.</t>
-  </si>
-  <si>
-    <t>SaaS</t>
-  </si>
-  <si>
-    <t>PaaS</t>
-  </si>
-  <si>
-    <t>Compatible with Ruby on Rails</t>
-  </si>
-  <si>
-    <t>As a product owner I want….</t>
-  </si>
-  <si>
-    <t>N 
-(.Net platform)</t>
-  </si>
-  <si>
-    <t>Restful API</t>
-  </si>
-  <si>
-    <t>Allows it to communicate with other services and components, using best practice protocols</t>
-  </si>
-  <si>
-    <t>As a product owner I want the CMS to be interoperable with other component and services so that the platform is extensible.</t>
-  </si>
-  <si>
-    <t>Graph QL</t>
-  </si>
-  <si>
-    <t>Query language for APIs</t>
-  </si>
-  <si>
-    <t>As a product owner I want be able to query the data held within the CMS so that I can search for specific information.</t>
-  </si>
-  <si>
-    <t>Supports webhooks</t>
-  </si>
-  <si>
-    <t>Provide real-time event driven information</t>
-  </si>
-  <si>
-    <t>As a product owner I want to use webhooks for my app or platform so that I can provide a real-time without developing an AP.</t>
-  </si>
-  <si>
-    <t>Y
-- Webhooks supported but functionality is limited below Enterprise level (e.g. not possible to trigger a webhook off certain "event" types). Templates and static webhook IPs provided in Enterprise version.</t>
-  </si>
-  <si>
-    <t>Integrations</t>
-  </si>
-  <si>
-    <t>Ability to interface and connect with other platforms and services</t>
-  </si>
-  <si>
-    <t>API</t>
-  </si>
-  <si>
-    <t>API
-- Integrates with martech technologies such as Marketo, Salesforce, Google Analytics, SEMrush, Brightcove, Watson, etc.
-- Integrations with Google Docs and Slack are being developed.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-- Integration with task management tools such as Trello, Jira and Asana in the roadmap
-- Delivery API not exposed in free Starter version.</t>
-  </si>
-  <si>
-    <t>API
-- Integrations with Slack being discussed but still in the roadmap</t>
-  </si>
-  <si>
-    <t>API
--Integration with a number of web services including Slack, GitHub, Google Analytics</t>
-  </si>
-  <si>
-    <t>Integrated with NEO for GraghQL interface/ Sparql (WC3 standard)</t>
-  </si>
-  <si>
-    <t>Notifications</t>
-  </si>
-  <si>
-    <t>Ability to send and receive messages in different applications</t>
-  </si>
-  <si>
-    <t>As a product owner I want to be able to send messages from the CMS so other platforms or service so that I can communicate with users.</t>
-  </si>
-  <si>
-    <t>Y
-- Notifications work in Slack as well as email</t>
-  </si>
-  <si>
-    <t>Content Previewing</t>
-  </si>
-  <si>
-    <t>To be able to preview content before it is published online</t>
-  </si>
-  <si>
-    <t>As a product owner I want I want to view my content before it is published online so that I can validate it is correct.</t>
-  </si>
-  <si>
-    <t>Rich Text Format Editor</t>
-  </si>
-  <si>
-    <t>Text formatting options</t>
-  </si>
-  <si>
-    <t>As a product owner I want to be able to format the text so that it is accessible for the audience.</t>
-  </si>
-  <si>
-    <t>Version History</t>
-  </si>
-  <si>
-    <t>To be able number and keep a log of historic releases</t>
-  </si>
-  <si>
-    <t>As a product owner I want to be able to view the history of published changes so that I have a record of past versions.</t>
-  </si>
-  <si>
-    <t>Scheduled Publishing</t>
-  </si>
-  <si>
-    <t>Ability to set the time content is to be published</t>
-  </si>
-  <si>
-    <t>As a product owner I want develop and release content at a plannned time so that content is published at the scheduled time.</t>
-  </si>
-  <si>
-    <t>Publishing Approval Workflow</t>
-  </si>
-  <si>
-    <t>Automated approval sign off for content before it is published</t>
-  </si>
-  <si>
-    <t>As a product owner I want changes to content to go through a business approval process so that the necessary checks are in place before publishing.</t>
-  </si>
-  <si>
-    <t>Workflow Tools</t>
-  </si>
-  <si>
-    <t>Ability to define processes and workflows to create, approve and publish content</t>
-  </si>
-  <si>
-    <t>- Content approval Workflows
-- Notifications only available in Enterprise plans
-- Custom roles only available in Enterprise plans
-- Content publishing and expiry scheduling only available in Enterprise plans
-- Content versioning and revision history for all plans</t>
-  </si>
-  <si>
-    <t>- Content publishing and expiry scheduling for all plans
-- Versioning and rollback
-- Built in approval workflows only available in Enterprise version
-- Ability to use webhooks for notifications limited below Enterprise
-- Grouped releases only available in Enterprise version</t>
-  </si>
-  <si>
-    <t>- Request review and approve content workflow (excluding free version)
-- Ability to leave comments and suggest changes for approval (excluding free version)
-- Built in notifications tool (email and Slack)
-- No limit on how webhooks are used for notifications
-- Revision history
-- Content publishing and expiry scheduling (excluding free version)
-- Dashboard view of assignments
-- Calendar view to see upcoming publishing or content expiry dates</t>
-  </si>
-  <si>
-    <t>- User roles limited to three (admin, publisher, writer) with no custom roles
-- Publishing workflow tool available in all plans
-- No limits on how webhooks are used for notifications
-- Release scheduling and bulk publishing for all plans
-- Full revision history</t>
-  </si>
-  <si>
-    <t>- Ability to build content publishing workflow for all plans
-- Zapier used for notifications
-- Scheduled publishing and expiry for all plans
-- Revision history for all plans</t>
-  </si>
-  <si>
-    <t>- Approval workflow tools and user permissions
-- Built in email notification tool
-- No limits on how webhooks are used for notifications
-- Content Publication &amp; Expiration Scheduling for all plans</t>
-  </si>
-  <si>
-    <t>Can develop and edit workflows</t>
-  </si>
-  <si>
-    <t>Multimedia Capability</t>
-  </si>
-  <si>
-    <t>Ability to Support media files such as images, videos, sound files etc</t>
-  </si>
-  <si>
-    <t>As a product owner I want to publish multimedia content so that I can give a rich user experience to the user.</t>
-  </si>
-  <si>
-    <t>- Wide variety of content modelling options- content types include text, dates, rich text, media (images, docs etc.), location, references to other content, arrays and even JSON for data.</t>
-  </si>
-  <si>
-    <t>- Supports all media files such as image link, video link, GIFs etc.
-- Maximum size of a single asset file is 700 MB (this can be restricted further using validation rules).</t>
-  </si>
-  <si>
-    <t>- Asset library supports a range of media types</t>
-  </si>
-  <si>
-    <t>- Every repository on Prismic has its own media library, which supports a range of file types including images, sounds files, videos, pdfs and more.
-- Max image size is 10Mb and max for any other file type is 100Mb
-- Imgix API used to make builds with images easier</t>
-  </si>
-  <si>
-    <t>- Supports a wide variety of media types including video.</t>
-  </si>
-  <si>
-    <t>No image manipulaton/ can use CDL</t>
-  </si>
-  <si>
-    <t>Secure Hosting</t>
-  </si>
-  <si>
-    <t>Hosting that is encrypted at rest and intransit and accessed securley (physical and digital). And hosted in a secure location.</t>
-  </si>
-  <si>
-    <t>As a product owner I want a secure service so that I can deliver content that is security compliant.</t>
-  </si>
-  <si>
-    <t>- Use AWS hosting</t>
-  </si>
-  <si>
-    <t>Multifactor Authentication</t>
-  </si>
-  <si>
-    <t>Enhanced authentication capability</t>
-  </si>
-  <si>
-    <t>As a product owner I want to keep access to the CMS platform secure so that only authorised user can access the platform.</t>
-  </si>
-  <si>
-    <t>Y
-- 2FA is an option even for the free tier but it is not enforced</t>
-  </si>
-  <si>
-    <t>Y
-For Enterprise Plans</t>
-  </si>
-  <si>
-    <t>Y
-Two factor authentication for Enterprise plans</t>
-  </si>
-  <si>
-    <t>- Two-factor authentication included for all plans.</t>
-  </si>
-  <si>
-    <t>- Windows and other authenticator options</t>
-  </si>
-  <si>
-    <t>Requires development and integration into identity provider</t>
-  </si>
-  <si>
-    <t>Security Certification</t>
-  </si>
-  <si>
-    <t>Provider is compliant with required standards</t>
-  </si>
-  <si>
-    <t>As a product owner I want the assurance that the CMS platform provider can demonstrate security compliance so that I know the platform will be secure to deliver my service.</t>
-  </si>
-  <si>
-    <t>Y 
-(ISO 27001:2013 compliant and ISO 27001 compliant data centres)</t>
-  </si>
-  <si>
-    <t>Y
-- SOC 2 Type II certification
-- ISO 27001 Compliant Data Centres - North American &amp; European Datacentres</t>
-  </si>
-  <si>
-    <t>- ISO 9001:2015, ISO 27001:2013 and ISO 20000-1:2011 certifications</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ISO/IEC 27001:2013, ISO/IEC 27017</t>
-  </si>
-  <si>
-    <t>- No ISO certifications</t>
-  </si>
-  <si>
-    <t>- Microsoft Azure infrastructure with ISO/IEC 27018, SOC 2 and more certifications</t>
-  </si>
-  <si>
-    <t>Pen tested by Fidus</t>
-  </si>
-  <si>
-    <t>Custom Roles</t>
-  </si>
-  <si>
-    <t>Ability to granularly control user access</t>
-  </si>
-  <si>
-    <t>As a product owner I want to be able to define user roles and permissions so that I can control levels of access to the CMS platform.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Custom roles only available in Enterprise plans</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Y
-In all plans
-</t>
-  </si>
-  <si>
-    <t>Custom roles for all plans</t>
-  </si>
-  <si>
-    <t>Pen Testing</t>
-  </si>
-  <si>
-    <t>Validate that that service has undertaken security assurances</t>
-  </si>
-  <si>
-    <t>As a product owner I want to know that the platform is regularly assessed for risks and vulnerabilities so that I know it is secure to deliver my service.</t>
-  </si>
-  <si>
-    <t>Y 
-(annual)</t>
-  </si>
-  <si>
-    <t>Y
-- Biannual Vulnerability Assessment and Penetration Testing (VAPT)</t>
-  </si>
-  <si>
-    <t>Annually</t>
-  </si>
-  <si>
-    <t>SSO</t>
-  </si>
-  <si>
-    <t>Ability to integrate with other identity services (e.g SAML 2.0 or Oauth)</t>
-  </si>
-  <si>
-    <t>As a product owner I want to be able to integrate my organisational SSO with the CMS platform so that users can use their corporate identity to access the platorm.</t>
-  </si>
-  <si>
-    <t>Only for enterprise plan</t>
-  </si>
-  <si>
-    <t>SSO with SAML 2.0</t>
-  </si>
-  <si>
-    <t>Single Sign-On for Enterprise plans</t>
-  </si>
-  <si>
-    <t>- Single-Sign-On for all plans</t>
-  </si>
-  <si>
-    <t>Third party sign on</t>
-  </si>
-  <si>
-    <t>Encryption (transit and rest)</t>
-  </si>
-  <si>
-    <t>Ensure all data is securley encrypted in transit and at rest (e.g TLS 1.2)</t>
-  </si>
-  <si>
-    <t>As a product owner I want to keep data secure when being transferred over a network so that we minimise data breaches and risk.</t>
-  </si>
-  <si>
-    <t>Y
-- 256-bit encryption of data in transit and at rest</t>
-  </si>
-  <si>
-    <t>- Data transferred between Prismic AWS EC2 instances and S3 storage facilities is secured via SSL endpoints using the HTTPS protocol. all Content Data is stored On disks in an encrypted manner (encrypted at rest)</t>
-  </si>
-  <si>
-    <t>- Data encryption at rest with 256-bit SSL encryption in transit</t>
-  </si>
-  <si>
-    <t>- Data transfer encryption (TLS 1.2)</t>
-  </si>
-  <si>
-    <t>Security Reporting</t>
-  </si>
-  <si>
-    <t>Insight report into security status and vulnerabilities of the service</t>
-  </si>
-  <si>
-    <t>As a product owner I want regular reports about the security health of the CMS platform so that I know it is secure and that vulnerabilities can be addressed.</t>
-  </si>
-  <si>
-    <t>Usage and activity reports</t>
-  </si>
-  <si>
-    <t>Uses Azure Monitoring</t>
-  </si>
-  <si>
-    <t>Data Soverignty</t>
-  </si>
-  <si>
-    <t>Location where the data is hosted and is subject to location data processsing policy and laws (e.g. GDPR)</t>
-  </si>
-  <si>
-    <t>As a product owner I want my service to be hosted in a secure compliant regional location so that I know my data and service will be secure by laws.</t>
-  </si>
-  <si>
-    <t>USA (Primary) &amp; EU (Backup)
-- Data is all hosted in North America, which could be an issue for any sensitive content</t>
-  </si>
-  <si>
-    <t>EU &amp; USA</t>
-  </si>
-  <si>
-    <t>Can choose - EU/USA/AUS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Data hosted in AWS facilities in Virginia, USA </t>
-  </si>
-  <si>
-    <t>Multi Region</t>
-  </si>
-  <si>
-    <t>On own infrastructure</t>
-  </si>
-  <si>
-    <t>Customer Support</t>
-  </si>
-  <si>
-    <t>First-line and technical support offered to the  organisation</t>
-  </si>
-  <si>
-    <t>As a product owner I want helpdesk support for the CMS platform so that if there any technical issues I can access support.</t>
-  </si>
-  <si>
-    <t>- Direct support only available for Enterprise plans.</t>
-  </si>
-  <si>
-    <t>Y
-- All Contentstack customers receive 24hr (Mon-Fri) support with average response times under 5 minutes. Enterprise plan includes 24/7 support.</t>
-  </si>
-  <si>
-    <t>Y
-- Priority chat and email for Business plan and 24/7x365 chat, email and phone for Enterprise
-- Service availability starts at 99.5% for Enterprise plans</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Y
-Priority Support in Platinum plan
-</t>
-  </si>
-  <si>
-    <t>-16h/day (Mon-Fri) in Professional plan</t>
-  </si>
-  <si>
-    <t>Y 
-(Community support)</t>
-  </si>
-  <si>
-    <t>Usability</t>
-  </si>
-  <si>
-    <t>Intuitive and easy to use with mininal training, configurable and accessible for users.</t>
-  </si>
-  <si>
-    <t>As a product owner I want the CMS platform to be easy to use so that I don't need specialist support.</t>
-  </si>
-  <si>
-    <t>- Simple to use WYSIWYG rich text editor
-- Simple content previewing</t>
-  </si>
-  <si>
-    <t>- WYSIWYG rich text editor
-- Content previewing requires publishing to a  "Preview" environment rather than there being a one click preview option (reducing the ease slightly)</t>
-  </si>
-  <si>
-    <t>- WYSIWYG rich text editor
-- Content previewing with in-browser editing</t>
-  </si>
-  <si>
-    <t>- WYSIWYG rich text editor
-- Drag and drop visual editing
-- Content previewing with in-browser editing feature
-- Page tagging and filtering</t>
-  </si>
-  <si>
-    <t>- WYSIWYG rich text editor
-- Content previewing</t>
-  </si>
-  <si>
-    <t>- WYSIWYG rich text editor
-- Content previewing including mobile devices
-- Drag and drop visual editing
-- Clean Copy &amp; Paste from Microsoft Word</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- WYSIWYG rich text editor
-</t>
-  </si>
-  <si>
-    <t>Uptime SLA's</t>
-  </si>
-  <si>
-    <t>Availablity and reliability of the service and how quick it is to recover and restore from and outage</t>
-  </si>
-  <si>
-    <t>As a product owner I want the CMS platform to have high availablity so that I can avoid a loss of service or downtime.</t>
-  </si>
-  <si>
-    <t>Y
-- SLA (99,9% API Uptime) 
-- 99.95% of API Uptime in Enterprise version</t>
-  </si>
-  <si>
-    <t>Y (99.9%)</t>
-  </si>
-  <si>
-    <t>PaaS dependent (by design)</t>
-  </si>
-  <si>
-    <t>Other Factors</t>
-  </si>
-  <si>
-    <t>Prices competitive at the mid and enterprise levels. Kontent is an option to give further consideration if looking to invest in the additional functionality that comes with a more premium plan.</t>
-  </si>
-  <si>
-    <t>Lack of ISO certifications rule this vendor out as an option at present. But the prices and features appear very competitive at this mid-level so Cosmic JS may be an option to reconsider in the future.</t>
-  </si>
-  <si>
-    <t>Not compatible with Ruby on Rails (.NET platform).
-Seems to be a decoupled rather than "API-first" headless CMS</t>
-  </si>
-  <si>
-    <t>Existing DfE Experience</t>
-  </si>
-  <si>
-    <t>As a product owner I want to reuse existing CMS patterns, templates and workflows so that I minimise the development time for my service.</t>
-  </si>
-  <si>
-    <t>-ILR
--Apprenticeship Fire it up
--Service Manual team</t>
-  </si>
-  <si>
-    <t>No known experience.</t>
-  </si>
-  <si>
-    <t>Used by National Careers Service team.</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2873,14 +2141,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -2935,7 +2195,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -3080,63 +2340,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3421,23 +2624,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:H31"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.44140625" customWidth="1"/>
-    <col min="2" max="2" width="29.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.33203125" style="14" customWidth="1"/>
-    <col min="4" max="4" width="68.88671875" style="14" customWidth="1"/>
+    <col min="1" max="1" width="5.42578125" customWidth="1"/>
+    <col min="2" max="2" width="29.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.28515625" style="14" customWidth="1"/>
+    <col min="4" max="4" width="68.85546875" style="14" customWidth="1"/>
     <col min="5" max="5" width="12" style="12" customWidth="1"/>
-    <col min="6" max="6" width="23.33203125" customWidth="1"/>
-    <col min="7" max="7" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.6640625" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" customWidth="1"/>
+    <col min="7" max="7" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="F2" s="3" t="s">
         <v>0</v>
       </c>
@@ -3448,7 +2651,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B3" s="16" t="s">
         <v>3</v>
       </c>
@@ -3465,7 +2668,7 @@
       <c r="G3" s="2"/>
       <c r="H3" s="32"/>
     </row>
-    <row r="4" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" s="17" t="s">
         <v>7</v>
       </c>
@@ -3488,7 +2691,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="17" t="s">
         <v>12</v>
       </c>
@@ -3511,7 +2714,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" s="17" t="s">
         <v>16</v>
       </c>
@@ -3534,7 +2737,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="17" t="s">
         <v>21</v>
       </c>
@@ -3557,7 +2760,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B8" s="17" t="s">
         <v>24</v>
       </c>
@@ -3580,7 +2783,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B9" s="17" t="s">
         <v>27</v>
       </c>
@@ -3603,7 +2806,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B10" s="17" t="s">
         <v>30</v>
       </c>
@@ -3626,7 +2829,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="19" t="s">
         <v>33</v>
       </c>
@@ -3637,7 +2840,7 @@
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
     </row>
-    <row r="12" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B12" s="17" t="s">
         <v>34</v>
       </c>
@@ -3660,7 +2863,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B13" s="17" t="s">
         <v>38</v>
       </c>
@@ -3683,7 +2886,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B14" s="17" t="s">
         <v>41</v>
       </c>
@@ -3706,7 +2909,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B15" s="17" t="s">
         <v>44</v>
       </c>
@@ -3729,7 +2932,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B16" s="17" t="s">
         <v>48</v>
       </c>
@@ -3752,7 +2955,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="17" t="s">
         <v>51</v>
       </c>
@@ -3775,7 +2978,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B18" s="17" t="s">
         <v>53</v>
       </c>
@@ -3798,7 +3001,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B19" s="17" t="s">
         <v>55</v>
       </c>
@@ -3821,7 +3024,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="19" t="s">
         <v>58</v>
       </c>
@@ -3832,7 +3035,7 @@
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
     </row>
-    <row r="21" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B21" s="17" t="s">
         <v>59</v>
       </c>
@@ -3855,7 +3058,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B22" s="17" t="s">
         <v>62</v>
       </c>
@@ -3878,7 +3081,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B23" s="17" t="s">
         <v>65</v>
       </c>
@@ -3901,7 +3104,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B24" s="17" t="s">
         <v>68</v>
       </c>
@@ -3924,7 +3127,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B25" s="17" t="s">
         <v>71</v>
       </c>
@@ -3947,7 +3150,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B26" s="17" t="s">
         <v>74</v>
       </c>
@@ -3970,7 +3173,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B27" s="17" t="s">
         <v>77</v>
       </c>
@@ -3993,7 +3196,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B28" s="17" t="s">
         <v>80</v>
       </c>
@@ -4016,7 +3219,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>83</v>
       </c>
@@ -4027,7 +3230,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>86</v>
       </c>
@@ -4046,18 +3249,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98D38F71-65DB-42D2-9179-80C1A6B69FBD}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:M32"/>
   <sheetViews>
@@ -4065,21 +3256,21 @@
       <selection activeCell="K43" sqref="K43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="35.88671875" customWidth="1"/>
-    <col min="4" max="5" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="35.85546875" customWidth="1"/>
+    <col min="4" max="5" width="28.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.6640625" customWidth="1"/>
+    <col min="7" max="7" width="24.7109375" customWidth="1"/>
     <col min="8" max="8" width="33" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="44.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.5546875" customWidth="1"/>
-    <col min="12" max="12" width="33.88671875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="44.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.5703125" customWidth="1"/>
+    <col min="12" max="12" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="35.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D2" s="5" t="s">
         <v>88</v>
       </c>
@@ -4111,7 +3302,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>97</v>
       </c>
@@ -4131,7 +3322,7 @@
       <c r="L3" s="7"/>
       <c r="M3" s="7"/>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>100</v>
       </c>
@@ -4167,7 +3358,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>102</v>
       </c>
@@ -4203,7 +3394,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
@@ -4219,7 +3410,7 @@
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
@@ -4235,7 +3426,7 @@
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>16</v>
       </c>
@@ -4255,7 +3446,7 @@
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>21</v>
       </c>
@@ -4275,7 +3466,7 @@
       <c r="L9" s="4"/>
       <c r="M9" s="4"/>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>24</v>
       </c>
@@ -4295,7 +3486,7 @@
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>27</v>
       </c>
@@ -4315,7 +3506,7 @@
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>30</v>
       </c>
@@ -4335,7 +3526,7 @@
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>33</v>
       </c>
@@ -4351,7 +3542,7 @@
       <c r="L13" s="5"/>
       <c r="M13" s="5"/>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>34</v>
       </c>
@@ -4371,7 +3562,7 @@
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>38</v>
       </c>
@@ -4391,7 +3582,7 @@
       <c r="L15" s="4"/>
       <c r="M15" s="4"/>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>41</v>
       </c>
@@ -4407,7 +3598,7 @@
       <c r="L16" s="4"/>
       <c r="M16" s="4"/>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>44</v>
       </c>
@@ -4423,7 +3614,7 @@
       <c r="L17" s="4"/>
       <c r="M17" s="4"/>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>48</v>
       </c>
@@ -4439,7 +3630,7 @@
       <c r="L18" s="4"/>
       <c r="M18" s="4"/>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>51</v>
       </c>
@@ -4455,7 +3646,7 @@
       <c r="L19" s="4"/>
       <c r="M19" s="4"/>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
         <v>53</v>
       </c>
@@ -4471,7 +3662,7 @@
       <c r="L20" s="4"/>
       <c r="M20" s="4"/>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>55</v>
       </c>
@@ -4491,7 +3682,7 @@
       <c r="L21" s="4"/>
       <c r="M21" s="4"/>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
         <v>58</v>
       </c>
@@ -4507,7 +3698,7 @@
       <c r="L22" s="5"/>
       <c r="M22" s="5"/>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
         <v>59</v>
       </c>
@@ -4523,7 +3714,7 @@
       <c r="L23" s="4"/>
       <c r="M23" s="4"/>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
         <v>62</v>
       </c>
@@ -4543,7 +3734,7 @@
       <c r="L24" s="4"/>
       <c r="M24" s="4"/>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
         <v>65</v>
       </c>
@@ -4563,7 +3754,7 @@
       <c r="L25" s="4"/>
       <c r="M25" s="4"/>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
         <v>68</v>
       </c>
@@ -4579,7 +3770,7 @@
       <c r="L26" s="4"/>
       <c r="M26" s="4"/>
     </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
         <v>71</v>
       </c>
@@ -4595,7 +3786,7 @@
       <c r="L27" s="4"/>
       <c r="M27" s="4"/>
     </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
         <v>74</v>
       </c>
@@ -4611,7 +3802,7 @@
       <c r="L28" s="4"/>
       <c r="M28" s="4"/>
     </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
         <v>77</v>
       </c>
@@ -4627,7 +3818,7 @@
       <c r="L29" s="4"/>
       <c r="M29" s="4"/>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
         <v>80</v>
       </c>
@@ -4643,7 +3834,7 @@
       <c r="L30" s="4"/>
       <c r="M30" s="4"/>
     </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
         <v>106</v>
       </c>
@@ -4659,7 +3850,7 @@
       <c r="L31" s="9"/>
       <c r="M31" s="9"/>
     </row>
-    <row r="32" spans="2:13" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="11" t="s">
         <v>107</v>
       </c>
@@ -4692,7 +3883,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:K17"/>
   <sheetViews>
@@ -4700,20 +3891,20 @@
       <selection activeCell="F4" sqref="F4:F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.6640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.44140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" style="27" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.33203125" customWidth="1"/>
-    <col min="8" max="9" width="24.6640625" customWidth="1"/>
-    <col min="10" max="10" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.6640625" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" style="27" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.28515625" customWidth="1"/>
+    <col min="8" max="9" width="24.7109375" customWidth="1"/>
+    <col min="10" max="10" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="F2" s="3" t="s">
         <v>113</v>
       </c>
@@ -4733,7 +3924,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>118</v>
       </c>
@@ -4755,7 +3946,7 @@
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:11" ht="45" x14ac:dyDescent="0.25">
       <c r="B4" s="11" t="s">
         <v>120</v>
       </c>
@@ -4787,7 +3978,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:11" ht="45" x14ac:dyDescent="0.25">
       <c r="B5" s="11" t="s">
         <v>123</v>
       </c>
@@ -4819,7 +4010,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="2:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:11" ht="60" x14ac:dyDescent="0.25">
       <c r="B6" s="11" t="s">
         <v>126</v>
       </c>
@@ -4851,7 +4042,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:11" ht="45" x14ac:dyDescent="0.25">
       <c r="B7" s="11" t="s">
         <v>129</v>
       </c>
@@ -4883,7 +4074,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:11" ht="45" x14ac:dyDescent="0.25">
       <c r="B8" s="11" t="s">
         <v>132</v>
       </c>
@@ -4915,7 +4106,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:11" ht="45" x14ac:dyDescent="0.25">
       <c r="B9" s="11" t="s">
         <v>135</v>
       </c>
@@ -4947,7 +4138,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:11" ht="45" x14ac:dyDescent="0.25">
       <c r="B10" s="11" t="s">
         <v>138</v>
       </c>
@@ -4979,7 +4170,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:11" ht="45" x14ac:dyDescent="0.25">
       <c r="B11" s="11" t="s">
         <v>141</v>
       </c>
@@ -5011,7 +4202,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:11" ht="45" x14ac:dyDescent="0.25">
       <c r="B12" s="11" t="s">
         <v>144</v>
       </c>
@@ -5043,7 +4234,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="2:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:11" ht="60" x14ac:dyDescent="0.25">
       <c r="B13" s="11" t="s">
         <v>147</v>
       </c>
@@ -5075,7 +4266,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:11" ht="45" x14ac:dyDescent="0.25">
       <c r="B14" s="11" t="s">
         <v>150</v>
       </c>
@@ -5107,7 +4298,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:11" ht="60" x14ac:dyDescent="0.25">
       <c r="B15" s="28" t="s">
         <v>153</v>
       </c>
@@ -5139,7 +4330,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D17" s="43"/>
     </row>
   </sheetData>
@@ -5148,7 +4339,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B2:J20"/>
   <sheetViews>
@@ -5156,20 +4347,20 @@
       <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="60.6640625" customWidth="1"/>
-    <col min="3" max="3" width="18.5546875" customWidth="1"/>
-    <col min="4" max="4" width="31.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.33203125" customWidth="1"/>
-    <col min="10" max="10" width="29.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="60.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" customWidth="1"/>
+    <col min="4" max="4" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.28515625" customWidth="1"/>
+    <col min="10" max="10" width="29.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C2" s="25" t="s">
         <v>157</v>
       </c>
@@ -5195,7 +4386,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
       <c r="E3" s="30"/>
@@ -5205,7 +4396,7 @@
       <c r="I3" s="30"/>
       <c r="J3" s="30"/>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C4" s="25"/>
       <c r="D4" s="25"/>
       <c r="E4" s="25"/>
@@ -5215,7 +4406,7 @@
       <c r="I4" s="25"/>
       <c r="J4" s="25"/>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C5" s="25" t="s">
         <v>104</v>
       </c>
@@ -5241,7 +4432,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>118</v>
       </c>
@@ -5254,7 +4445,7 @@
       <c r="I6" s="23"/>
       <c r="J6" s="23"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="11" t="s">
         <v>120</v>
       </c>
@@ -5267,7 +4458,7 @@
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="11" t="s">
         <v>123</v>
       </c>
@@ -5280,7 +4471,7 @@
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" s="11" t="s">
         <v>126</v>
       </c>
@@ -5293,7 +4484,7 @@
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="11" t="s">
         <v>129</v>
       </c>
@@ -5306,7 +4497,7 @@
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="11" t="s">
         <v>132</v>
       </c>
@@ -5319,7 +4510,7 @@
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" s="11" t="s">
         <v>135</v>
       </c>
@@ -5332,7 +4523,7 @@
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" s="11" t="s">
         <v>138</v>
       </c>
@@ -5345,7 +4536,7 @@
       <c r="I13" s="29"/>
       <c r="J13" s="29"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="11" t="s">
         <v>141</v>
       </c>
@@ -5358,7 +4549,7 @@
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" s="11" t="s">
         <v>144</v>
       </c>
@@ -5371,7 +4562,7 @@
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" s="11" t="s">
         <v>147</v>
       </c>
@@ -5384,7 +4575,7 @@
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="11" t="s">
         <v>150</v>
       </c>
@@ -5397,7 +4588,7 @@
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="28" t="s">
         <v>153</v>
       </c>
@@ -5410,7 +4601,7 @@
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
         <v>106</v>
       </c>
@@ -5423,7 +4614,7 @@
       <c r="I19" s="9"/>
       <c r="J19" s="9"/>
     </row>
-    <row r="20" spans="2:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:10" ht="60" x14ac:dyDescent="0.25">
       <c r="B20" s="11" t="s">
         <v>107</v>
       </c>
@@ -5446,7 +4637,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B2:M19"/>
   <sheetViews>
@@ -5454,22 +4645,22 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31" style="42" customWidth="1"/>
     <col min="4" max="4" width="47" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.88671875" customWidth="1"/>
-    <col min="8" max="8" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.88671875" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" customWidth="1"/>
+    <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.85546875" customWidth="1"/>
     <col min="10" max="10" width="19" customWidth="1"/>
-    <col min="11" max="11" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.33203125" customWidth="1"/>
+    <col min="11" max="11" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B2" s="33"/>
       <c r="C2" s="40"/>
       <c r="D2" s="35"/>
@@ -5497,7 +4688,7 @@
       </c>
       <c r="M2" s="33"/>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B3" s="33"/>
       <c r="C3" s="40"/>
       <c r="D3" s="35"/>
@@ -5525,7 +4716,7 @@
       </c>
       <c r="M3" s="33"/>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B4" s="33"/>
       <c r="C4" s="40"/>
       <c r="D4" s="35"/>
@@ -5539,7 +4730,7 @@
       <c r="L4" s="34"/>
       <c r="M4" s="33"/>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5" s="34" t="s">
         <v>177</v>
       </c>
@@ -5561,7 +4752,7 @@
       <c r="L5" s="34"/>
       <c r="M5" s="33"/>
     </row>
-    <row r="6" spans="2:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:13" ht="45" x14ac:dyDescent="0.25">
       <c r="B6" s="17" t="s">
         <v>178</v>
       </c>
@@ -5597,7 +4788,7 @@
       </c>
       <c r="M6" s="33"/>
     </row>
-    <row r="7" spans="2:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:13" ht="45" x14ac:dyDescent="0.25">
       <c r="B7" s="17" t="s">
         <v>182</v>
       </c>
@@ -5633,7 +4824,7 @@
       </c>
       <c r="M7" s="33"/>
     </row>
-    <row r="8" spans="2:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:13" ht="45" x14ac:dyDescent="0.25">
       <c r="B8" s="17" t="s">
         <v>185</v>
       </c>
@@ -5669,7 +4860,7 @@
       </c>
       <c r="M8" s="33"/>
     </row>
-    <row r="9" spans="2:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:13" ht="45" x14ac:dyDescent="0.25">
       <c r="B9" s="17" t="s">
         <v>169</v>
       </c>
@@ -5705,7 +4896,7 @@
       </c>
       <c r="M9" s="33"/>
     </row>
-    <row r="10" spans="2:13" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:13" ht="75" x14ac:dyDescent="0.25">
       <c r="B10" s="17" t="s">
         <v>190</v>
       </c>
@@ -5741,7 +4932,7 @@
       </c>
       <c r="M10" s="33"/>
     </row>
-    <row r="11" spans="2:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:13" ht="45" x14ac:dyDescent="0.25">
       <c r="B11" s="17" t="s">
         <v>193</v>
       </c>
@@ -5777,7 +4968,7 @@
       </c>
       <c r="M11" s="33"/>
     </row>
-    <row r="12" spans="2:13" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:13" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="17" t="s">
         <v>196</v>
       </c>
@@ -5813,7 +5004,7 @@
       </c>
       <c r="M12" s="33"/>
     </row>
-    <row r="13" spans="2:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:13" ht="45" x14ac:dyDescent="0.25">
       <c r="B13" s="17" t="s">
         <v>200</v>
       </c>
@@ -5849,7 +5040,7 @@
       </c>
       <c r="M13" s="33"/>
     </row>
-    <row r="14" spans="2:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:13" ht="45" x14ac:dyDescent="0.25">
       <c r="B14" s="17" t="s">
         <v>203</v>
       </c>
@@ -5885,7 +5076,7 @@
       </c>
       <c r="M14" s="33"/>
     </row>
-    <row r="15" spans="2:13" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:13" ht="60" x14ac:dyDescent="0.25">
       <c r="B15" s="17" t="s">
         <v>207</v>
       </c>
@@ -5921,7 +5112,7 @@
       </c>
       <c r="M15" s="33"/>
     </row>
-    <row r="16" spans="2:13" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:13" ht="60" x14ac:dyDescent="0.25">
       <c r="B16" s="17" t="s">
         <v>211</v>
       </c>
@@ -5957,7 +5148,7 @@
       </c>
       <c r="M16" s="33"/>
     </row>
-    <row r="17" spans="2:13" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:13" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="17" t="s">
         <v>214</v>
       </c>
@@ -5993,7 +5184,7 @@
       </c>
       <c r="M17" s="33"/>
     </row>
-    <row r="18" spans="2:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:13" ht="45" x14ac:dyDescent="0.25">
       <c r="B18" s="17" t="s">
         <v>217</v>
       </c>
@@ -6029,7 +5220,7 @@
       </c>
       <c r="M18" s="33"/>
     </row>
-    <row r="19" spans="2:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:13" ht="45" x14ac:dyDescent="0.25">
       <c r="B19" s="37" t="s">
         <v>220</v>
       </c>
@@ -6071,7 +5262,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="B2:P23"/>
   <sheetViews>
@@ -6079,19 +5270,19 @@
       <selection activeCell="P1" sqref="P1:P1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.88671875" customWidth="1"/>
-    <col min="5" max="5" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.88671875" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" customWidth="1"/>
     <col min="7" max="7" width="19" customWidth="1"/>
-    <col min="8" max="8" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="15" width="20.33203125" customWidth="1"/>
+    <col min="8" max="8" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="15" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" s="44" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:16" s="44" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="36" t="s">
         <v>223</v>
       </c>
@@ -6132,7 +5323,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B3" s="33"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -6149,7 +5340,7 @@
       <c r="O3" s="5"/>
       <c r="P3" s="33"/>
     </row>
-    <row r="4" spans="2:16" s="46" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:16" s="46" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="C4" s="25" t="s">
         <v>168</v>
       </c>
@@ -6190,7 +5381,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="34" t="s">
         <v>118</v>
       </c>
@@ -6209,7 +5400,7 @@
       <c r="O5" s="34"/>
       <c r="P5" s="33"/>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" s="17" t="s">
         <v>178</v>
       </c>
@@ -6232,7 +5423,7 @@
       <c r="O6" s="4"/>
       <c r="P6" s="33"/>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B7" s="17" t="s">
         <v>182</v>
       </c>
@@ -6255,7 +5446,7 @@
       <c r="O7" s="4"/>
       <c r="P7" s="33"/>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B8" s="17" t="s">
         <v>185</v>
       </c>
@@ -6278,7 +5469,7 @@
       <c r="O8" s="4"/>
       <c r="P8" s="33"/>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B9" s="17" t="s">
         <v>169</v>
       </c>
@@ -6301,7 +5492,7 @@
       <c r="O9" s="4"/>
       <c r="P9" s="33"/>
     </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B10" s="17" t="s">
         <v>190</v>
       </c>
@@ -6324,7 +5515,7 @@
       <c r="O10" s="4"/>
       <c r="P10" s="33"/>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B11" s="17" t="s">
         <v>193</v>
       </c>
@@ -6347,7 +5538,7 @@
       <c r="O11" s="4"/>
       <c r="P11" s="33"/>
     </row>
-    <row r="12" spans="2:16" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:16" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B12" s="17" t="s">
         <v>196</v>
       </c>
@@ -6370,7 +5561,7 @@
       <c r="O12" s="10"/>
       <c r="P12" s="33"/>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B13" s="17" t="s">
         <v>200</v>
       </c>
@@ -6393,7 +5584,7 @@
       <c r="O13" s="4"/>
       <c r="P13" s="33"/>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B14" s="17" t="s">
         <v>203</v>
       </c>
@@ -6416,7 +5607,7 @@
       <c r="O14" s="10"/>
       <c r="P14" s="33"/>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B15" s="17" t="s">
         <v>207</v>
       </c>
@@ -6439,7 +5630,7 @@
       <c r="O15" s="4"/>
       <c r="P15" s="33"/>
     </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B16" s="17" t="s">
         <v>211</v>
       </c>
@@ -6462,7 +5653,7 @@
       <c r="O16" s="4"/>
       <c r="P16" s="33"/>
     </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B17" s="17" t="s">
         <v>214</v>
       </c>
@@ -6485,7 +5676,7 @@
       <c r="O17" s="4"/>
       <c r="P17" s="33"/>
     </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B18" s="17" t="s">
         <v>217</v>
       </c>
@@ -6508,7 +5699,7 @@
       <c r="O18" s="4"/>
       <c r="P18" s="33"/>
     </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B19" s="37" t="s">
         <v>220</v>
       </c>
@@ -6531,22 +5722,22 @@
       <c r="O19" s="4"/>
       <c r="P19" s="33"/>
     </row>
-    <row r="20" spans="2:16" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:16" ht="135" x14ac:dyDescent="0.25">
       <c r="K20" s="48" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="21" spans="2:16" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:16" ht="90" x14ac:dyDescent="0.25">
       <c r="K21" s="49" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="22" spans="2:16" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:16" ht="45" x14ac:dyDescent="0.25">
       <c r="K22" s="50" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="23" spans="2:16" ht="72" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:16" ht="75" x14ac:dyDescent="0.25">
       <c r="K23" s="50" t="s">
         <v>244</v>
       </c>
@@ -6562,1085 +5753,22 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77CFD866-DE87-41D5-BE31-43FB6D2DE716}">
-  <dimension ref="B2:L32"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="28.77734375" style="68" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.88671875" style="14" customWidth="1"/>
-    <col min="4" max="4" width="38.21875" customWidth="1"/>
-    <col min="5" max="5" width="9.109375" customWidth="1"/>
-    <col min="6" max="6" width="31.44140625" customWidth="1"/>
-    <col min="7" max="7" width="28.6640625" customWidth="1"/>
-    <col min="8" max="8" width="36.5546875" customWidth="1"/>
-    <col min="9" max="10" width="30.21875" customWidth="1"/>
-    <col min="11" max="11" width="34.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="31.21875" style="69" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:12" s="14" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B2" s="15" t="s">
-        <v>245</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="36" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="36" t="s">
-        <v>246</v>
-      </c>
-      <c r="G2" s="36" t="s">
-        <v>247</v>
-      </c>
-      <c r="H2" s="36" t="s">
-        <v>248</v>
-      </c>
-      <c r="I2" s="36" t="s">
-        <v>249</v>
-      </c>
-      <c r="J2" s="36" t="s">
-        <v>250</v>
-      </c>
-      <c r="K2" s="36" t="s">
-        <v>251</v>
-      </c>
-      <c r="L2" s="36" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B3" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="52" t="s">
-        <v>254</v>
-      </c>
-      <c r="G3" s="53" t="s">
-        <v>255</v>
-      </c>
-      <c r="H3" s="52" t="s">
-        <v>256</v>
-      </c>
-      <c r="I3" s="52" t="s">
-        <v>257</v>
-      </c>
-      <c r="J3" s="52" t="s">
-        <v>258</v>
-      </c>
-      <c r="K3" s="52" t="s">
-        <v>259</v>
-      </c>
-      <c r="L3" s="54" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="4" spans="2:12" ht="409.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="55" t="s">
-        <v>261</v>
-      </c>
-      <c r="C4" s="51"/>
-      <c r="D4" s="56" t="s">
-        <v>262</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="18" t="s">
-        <v>263</v>
-      </c>
-      <c r="G4" s="18" t="s">
-        <v>264</v>
-      </c>
-      <c r="H4" s="40" t="s">
-        <v>265</v>
-      </c>
-      <c r="I4" s="57" t="s">
-        <v>266</v>
-      </c>
-      <c r="J4" s="57" t="s">
-        <v>267</v>
-      </c>
-      <c r="K4" s="18" t="s">
-        <v>268</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="5" spans="2:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B5" s="55" t="s">
-        <v>270</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>271</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>272</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>273</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>273</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>273</v>
-      </c>
-      <c r="I5" s="10" t="s">
-        <v>273</v>
-      </c>
-      <c r="J5" s="10" t="s">
-        <v>273</v>
-      </c>
-      <c r="K5" s="10" t="s">
-        <v>273</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="6" spans="2:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="55" t="s">
-        <v>275</v>
-      </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13" t="s">
-        <v>276</v>
-      </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="K6" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="L6" s="4"/>
-    </row>
-    <row r="7" spans="2:12" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B7" s="55" t="s">
-        <v>278</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>279</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>280</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="L7" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="2:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B8" s="55" t="s">
-        <v>281</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>282</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>283</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="K8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="L8" s="10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="2:12" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="B9" s="55" t="s">
-        <v>284</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>285</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>286</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>287</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="K9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="L9" s="10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="2:12" ht="145.94999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="17" t="s">
-        <v>288</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>289</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>280</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>290</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>291</v>
-      </c>
-      <c r="H10" s="10" t="s">
-        <v>292</v>
-      </c>
-      <c r="I10" s="10" t="s">
-        <v>293</v>
-      </c>
-      <c r="J10" s="10" t="s">
-        <v>294</v>
-      </c>
-      <c r="K10" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="L10" s="10" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="11" spans="2:12" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B11" s="55" t="s">
-        <v>296</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>297</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>298</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G11" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="H11" s="10" t="s">
-        <v>299</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="K11" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="L11" s="58" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="2:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B12" s="55" t="s">
-        <v>300</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>301</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>302</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J12" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="K12" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="L12" s="58" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="2:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B13" s="55" t="s">
-        <v>303</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>304</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>305</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="K13" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="L13" s="59" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="2:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B14" s="55" t="s">
-        <v>306</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>307</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>308</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I14" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J14" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="K14" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="L14" s="58" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="2:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B15" s="11" t="s">
-        <v>309</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>310</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>311</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I15" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J15" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="K15" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="L15" s="59" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="2:12" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B16" s="17" t="s">
-        <v>312</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>313</v>
-      </c>
-      <c r="D16" s="13" t="s">
-        <v>314</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="G16" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="H16" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="I16" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="J16" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="K16" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="L16" s="59" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="2:12" ht="270.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="17" t="s">
-        <v>315</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>316</v>
-      </c>
-      <c r="D17" s="13" t="s">
-        <v>314</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F17" s="60" t="s">
-        <v>317</v>
-      </c>
-      <c r="G17" s="61" t="s">
-        <v>318</v>
-      </c>
-      <c r="H17" s="61" t="s">
-        <v>319</v>
-      </c>
-      <c r="I17" s="61" t="s">
-        <v>320</v>
-      </c>
-      <c r="J17" s="61" t="s">
-        <v>321</v>
-      </c>
-      <c r="K17" s="61" t="s">
-        <v>322</v>
-      </c>
-      <c r="L17" s="62" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="18" spans="2:12" ht="166.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="18" t="s">
-        <v>324</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>325</v>
-      </c>
-      <c r="D18" s="13" t="s">
-        <v>326</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F18" s="61" t="s">
-        <v>327</v>
-      </c>
-      <c r="G18" s="61" t="s">
-        <v>328</v>
-      </c>
-      <c r="H18" s="61" t="s">
-        <v>329</v>
-      </c>
-      <c r="I18" s="61" t="s">
-        <v>330</v>
-      </c>
-      <c r="J18" s="61" t="s">
-        <v>329</v>
-      </c>
-      <c r="K18" s="61" t="s">
-        <v>331</v>
-      </c>
-      <c r="L18" s="62" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="19" spans="2:12" ht="72" x14ac:dyDescent="0.3">
-      <c r="B19" s="13" t="s">
-        <v>333</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>334</v>
-      </c>
-      <c r="D19" s="13" t="s">
-        <v>335</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I19" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J19" s="63" t="s">
-        <v>336</v>
-      </c>
-      <c r="K19" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="L19" s="59" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="20" spans="2:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B20" s="11" t="s">
-        <v>337</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>338</v>
-      </c>
-      <c r="D20" s="13" t="s">
-        <v>339</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F20" s="10" t="s">
-        <v>340</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H20" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="I20" s="10" t="s">
-        <v>342</v>
-      </c>
-      <c r="J20" s="64" t="s">
-        <v>343</v>
-      </c>
-      <c r="K20" s="64" t="s">
-        <v>344</v>
-      </c>
-      <c r="L20" s="59" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="21" spans="2:12" ht="72" x14ac:dyDescent="0.3">
-      <c r="B21" s="11" t="s">
-        <v>346</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>347</v>
-      </c>
-      <c r="D21" s="13" t="s">
-        <v>348</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F21" s="65" t="s">
-        <v>349</v>
-      </c>
-      <c r="G21" s="65" t="s">
-        <v>350</v>
-      </c>
-      <c r="H21" s="65" t="s">
-        <v>351</v>
-      </c>
-      <c r="I21" s="65" t="s">
-        <v>352</v>
-      </c>
-      <c r="J21" s="66" t="s">
-        <v>353</v>
-      </c>
-      <c r="K21" s="67" t="s">
-        <v>354</v>
-      </c>
-      <c r="L21" s="62" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="22" spans="2:12" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B22" s="17" t="s">
-        <v>356</v>
-      </c>
-      <c r="C22" s="13" t="s">
-        <v>357</v>
-      </c>
-      <c r="D22" s="13" t="s">
-        <v>358</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F22" s="10" t="s">
-        <v>359</v>
-      </c>
-      <c r="G22" s="10" t="s">
-        <v>360</v>
-      </c>
-      <c r="H22" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I22" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="J22" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="K22" s="4" t="s">
-        <v>361</v>
-      </c>
-      <c r="L22" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="23" spans="2:12" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B23" s="11" t="s">
-        <v>362</v>
-      </c>
-      <c r="C23" s="13" t="s">
-        <v>363</v>
-      </c>
-      <c r="D23" s="13" t="s">
-        <v>364</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F23" s="10" t="s">
-        <v>365</v>
-      </c>
-      <c r="G23" s="64" t="s">
-        <v>366</v>
-      </c>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4" t="s">
-        <v>367</v>
-      </c>
-      <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
-      <c r="L23" s="10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="24" spans="2:12" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B24" s="11" t="s">
-        <v>368</v>
-      </c>
-      <c r="C24" s="13" t="s">
-        <v>369</v>
-      </c>
-      <c r="D24" s="13" t="s">
-        <v>370</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>371</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>372</v>
-      </c>
-      <c r="H24" s="4" t="s">
-        <v>373</v>
-      </c>
-      <c r="I24" s="4" t="s">
-        <v>373</v>
-      </c>
-      <c r="J24" s="4" t="s">
-        <v>372</v>
-      </c>
-      <c r="K24" s="63" t="s">
-        <v>374</v>
-      </c>
-      <c r="L24" s="59" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="25" spans="2:12" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="B25" s="13" t="s">
-        <v>376</v>
-      </c>
-      <c r="C25" s="13" t="s">
-        <v>377</v>
-      </c>
-      <c r="D25" s="13" t="s">
-        <v>378</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G25" s="10" t="s">
-        <v>379</v>
-      </c>
-      <c r="H25" s="4"/>
-      <c r="I25" s="64" t="s">
-        <v>380</v>
-      </c>
-      <c r="J25" s="64" t="s">
-        <v>381</v>
-      </c>
-      <c r="K25" s="63" t="s">
-        <v>382</v>
-      </c>
-      <c r="L25" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="26" spans="2:12" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B26" s="11" t="s">
-        <v>383</v>
-      </c>
-      <c r="C26" s="13" t="s">
-        <v>384</v>
-      </c>
-      <c r="D26" s="13" t="s">
-        <v>385</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="4"/>
-      <c r="J26" s="4" t="s">
-        <v>386</v>
-      </c>
-      <c r="K26" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="L26" s="59" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="27" spans="2:12" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B27" s="11" t="s">
-        <v>388</v>
-      </c>
-      <c r="C27" s="13" t="s">
-        <v>389</v>
-      </c>
-      <c r="D27" s="13" t="s">
-        <v>390</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F27" s="10" t="s">
-        <v>391</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>392</v>
-      </c>
-      <c r="H27" s="4" t="s">
-        <v>393</v>
-      </c>
-      <c r="I27" s="64" t="s">
-        <v>394</v>
-      </c>
-      <c r="J27" s="4" t="s">
-        <v>395</v>
-      </c>
-      <c r="K27" s="4" t="s">
-        <v>395</v>
-      </c>
-      <c r="L27" s="4" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="28" spans="2:12" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="B28" s="11" t="s">
-        <v>397</v>
-      </c>
-      <c r="C28" s="13" t="s">
-        <v>398</v>
-      </c>
-      <c r="D28" s="13" t="s">
-        <v>399</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F28" s="61" t="s">
-        <v>400</v>
-      </c>
-      <c r="G28" s="10" t="s">
-        <v>401</v>
-      </c>
-      <c r="H28" s="10" t="s">
-        <v>402</v>
-      </c>
-      <c r="I28" s="10" t="s">
-        <v>403</v>
-      </c>
-      <c r="J28" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="K28" s="63" t="s">
-        <v>404</v>
-      </c>
-      <c r="L28" s="10" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="29" spans="2:12" ht="119.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="17" t="s">
-        <v>406</v>
-      </c>
-      <c r="C29" s="13" t="s">
-        <v>407</v>
-      </c>
-      <c r="D29" s="13" t="s">
-        <v>408</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F29" s="61" t="s">
-        <v>409</v>
-      </c>
-      <c r="G29" s="61" t="s">
-        <v>410</v>
-      </c>
-      <c r="H29" s="61" t="s">
-        <v>411</v>
-      </c>
-      <c r="I29" s="61" t="s">
-        <v>412</v>
-      </c>
-      <c r="J29" s="61" t="s">
-        <v>413</v>
-      </c>
-      <c r="K29" s="61" t="s">
-        <v>414</v>
-      </c>
-      <c r="L29" s="61" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="30" spans="2:12" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B30" s="11" t="s">
-        <v>416</v>
-      </c>
-      <c r="C30" s="13" t="s">
-        <v>417</v>
-      </c>
-      <c r="D30" s="13" t="s">
-        <v>418</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H30" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I30" s="10" t="s">
-        <v>419</v>
-      </c>
-      <c r="J30" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="K30" s="4" t="s">
-        <v>420</v>
-      </c>
-      <c r="L30" s="10" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="31" spans="2:12" ht="112.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="11" t="s">
-        <v>422</v>
-      </c>
-      <c r="C31" s="51"/>
-      <c r="D31" s="51"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="18" t="s">
-        <v>423</v>
-      </c>
-      <c r="I31" s="4"/>
-      <c r="J31" s="18" t="s">
-        <v>424</v>
-      </c>
-      <c r="K31" s="61" t="s">
-        <v>425</v>
-      </c>
-      <c r="L31" s="58"/>
-    </row>
-    <row r="32" spans="2:12" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B32" s="11" t="s">
-        <v>426</v>
-      </c>
-      <c r="C32" s="51"/>
-      <c r="D32" s="13" t="s">
-        <v>427</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F32" s="64" t="s">
-        <v>428</v>
-      </c>
-      <c r="G32" s="4" t="s">
-        <v>429</v>
-      </c>
-      <c r="H32" s="4" t="s">
-        <v>429</v>
-      </c>
-      <c r="I32" s="4" t="s">
-        <v>429</v>
-      </c>
-      <c r="J32" s="4" t="s">
-        <v>429</v>
-      </c>
-      <c r="K32" s="4" t="s">
-        <v>430</v>
-      </c>
-      <c r="L32" s="10" t="s">
-        <v>430</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="F3" r:id="rId1" xr:uid="{71BC4B22-CCEF-4EA5-8A95-5A3A4D4B5EF9}"/>
-    <hyperlink ref="G3" r:id="rId2" xr:uid="{4F8CB76F-DCE3-43A8-97FB-7E485E0FC38D}"/>
-    <hyperlink ref="K3" r:id="rId3" xr:uid="{23C6D77B-538B-40AB-A6D4-772DDEB582BE}"/>
-    <hyperlink ref="I3" r:id="rId4" xr:uid="{55ED426A-5DA9-4E47-A769-89669434E55B}"/>
-    <hyperlink ref="H3" r:id="rId5" xr:uid="{FCB86B0D-9681-4F78-AD71-C398F6C5B7D4}"/>
-    <hyperlink ref="J3" r:id="rId6" xr:uid="{46F94EBA-7865-48C6-B065-4D110AE97818}"/>
-    <hyperlink ref="L3" r:id="rId7" xr:uid="{B6ABF243-587B-4246-8761-BB7C0832C12D}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId8"/>
-</worksheet>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B57151A7873D3B4CB38449F1E4CD2EAA" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7e8202c7bfeeae60ce525a5ca4d0fe6a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="161ae125-8199-47a3-b5d9-eda3a8f2a061" xmlns:ns4="680bcac6-b14c-4c2b-a58b-c019311aeaad" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1abf75ed68cd583d13418a16f207a9e6" ns3:_="" ns4:_="">
     <xsd:import namespace="161ae125-8199-47a3-b5d9-eda3a8f2a061"/>
@@ -7843,36 +5971,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4651E139-BFC7-495A-9CCD-06709AD31B99}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FBD369E-6A68-4C96-8DEA-0EC45C5264AD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="161ae125-8199-47a3-b5d9-eda3a8f2a061"/>
-    <ds:schemaRef ds:uri="680bcac6-b14c-4c2b-a58b-c019311aeaad"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -7895,9 +5997,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FBD369E-6A68-4C96-8DEA-0EC45C5264AD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4651E139-BFC7-495A-9CCD-06709AD31B99}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="161ae125-8199-47a3-b5d9-eda3a8f2a061"/>
+    <ds:schemaRef ds:uri="680bcac6-b14c-4c2b-a58b-c019311aeaad"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>